<commit_message>
Last try with Plotly
</commit_message>
<xml_diff>
--- a/data/food/inseguridad por barrio 2022 data.xlsx
+++ b/data/food/inseguridad por barrio 2022 data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kei\Documents\GitHub\FS-Security\data\food\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BFF4FA-926C-44C0-A542-D6BBF842B29E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F7402E-4022-46E1-ABCE-81A2E5CED545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5001,9 +5001,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5320,7 +5321,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M940"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5403,7 +5406,7 @@
       <c r="H2">
         <v>0.39</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="2">
         <v>38.79</v>
       </c>
       <c r="J2">
@@ -5444,7 +5447,7 @@
       <c r="H3">
         <v>0.46</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="2">
         <v>46.18</v>
       </c>
       <c r="J3">
@@ -5485,7 +5488,7 @@
       <c r="H4">
         <v>0.39</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="2">
         <v>38.630000000000003</v>
       </c>
       <c r="J4">
@@ -5526,7 +5529,7 @@
       <c r="H5">
         <v>0.4</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="2">
         <v>39.659999999999997</v>
       </c>
       <c r="J5">
@@ -5567,7 +5570,7 @@
       <c r="H6">
         <v>0.36</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="2">
         <v>35.880000000000003</v>
       </c>
       <c r="J6">
@@ -5608,7 +5611,7 @@
       <c r="H7">
         <v>0.51</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="2">
         <v>50.63</v>
       </c>
       <c r="J7">
@@ -5649,7 +5652,7 @@
       <c r="H8">
         <v>0.54</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="2">
         <v>53.77</v>
       </c>
       <c r="J8">
@@ -5690,7 +5693,7 @@
       <c r="H9">
         <v>0.39</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="2">
         <v>39.380000000000003</v>
       </c>
       <c r="J9">
@@ -5731,7 +5734,7 @@
       <c r="H10">
         <v>0.36</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="2">
         <v>35.69</v>
       </c>
       <c r="J10">
@@ -5772,7 +5775,7 @@
       <c r="H11">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="2">
         <v>29.49</v>
       </c>
       <c r="J11">
@@ -5813,7 +5816,7 @@
       <c r="H12">
         <v>0.41</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="2">
         <v>41.48</v>
       </c>
       <c r="J12">
@@ -5854,7 +5857,7 @@
       <c r="H13">
         <v>0.34</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="2">
         <v>34.119999999999997</v>
       </c>
       <c r="J13">
@@ -5895,7 +5898,7 @@
       <c r="H14">
         <v>0.32</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="2">
         <v>31.69</v>
       </c>
       <c r="J14">
@@ -5936,7 +5939,7 @@
       <c r="H15">
         <v>0.45</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="2">
         <v>44.57</v>
       </c>
       <c r="J15">
@@ -5977,7 +5980,7 @@
       <c r="H16">
         <v>0.32</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="2">
         <v>32.32</v>
       </c>
       <c r="J16">
@@ -6018,7 +6021,7 @@
       <c r="H17">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="2">
         <v>29.4</v>
       </c>
       <c r="J17">
@@ -6059,7 +6062,7 @@
       <c r="H18">
         <v>0.38</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="2">
         <v>38.340000000000003</v>
       </c>
       <c r="J18">
@@ -6100,7 +6103,7 @@
       <c r="H19">
         <v>0</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="2">
         <v>0</v>
       </c>
       <c r="J19">
@@ -6135,7 +6138,7 @@
       <c r="H20">
         <v>0.33</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="2">
         <v>32.78</v>
       </c>
       <c r="J20">
@@ -6176,7 +6179,7 @@
       <c r="H21">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="2">
         <v>28.23</v>
       </c>
       <c r="J21">
@@ -6217,7 +6220,7 @@
       <c r="H22">
         <v>0.39</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="2">
         <v>39.36</v>
       </c>
       <c r="J22">
@@ -6258,7 +6261,7 @@
       <c r="H23">
         <v>0.43</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="2">
         <v>43.03</v>
       </c>
       <c r="J23">
@@ -6299,7 +6302,7 @@
       <c r="H24">
         <v>0.38</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="2">
         <v>38.090000000000003</v>
       </c>
       <c r="J24">
@@ -6340,7 +6343,7 @@
       <c r="H25">
         <v>0.32</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="2">
         <v>32.28</v>
       </c>
       <c r="J25">
@@ -6381,7 +6384,7 @@
       <c r="H26">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="2">
         <v>29.18</v>
       </c>
       <c r="J26">
@@ -6422,7 +6425,7 @@
       <c r="H27">
         <v>0.3</v>
       </c>
-      <c r="I27">
+      <c r="I27" s="2">
         <v>30.07</v>
       </c>
       <c r="J27">
@@ -6463,7 +6466,7 @@
       <c r="H28">
         <v>0.37</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="2">
         <v>37.39</v>
       </c>
       <c r="J28">
@@ -6504,7 +6507,7 @@
       <c r="H29">
         <v>0.27</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="2">
         <v>26.55</v>
       </c>
       <c r="J29">
@@ -6545,7 +6548,7 @@
       <c r="H30">
         <v>0.33</v>
       </c>
-      <c r="I30">
+      <c r="I30" s="2">
         <v>32.58</v>
       </c>
       <c r="J30">
@@ -6586,7 +6589,7 @@
       <c r="H31">
         <v>0.31</v>
       </c>
-      <c r="I31">
+      <c r="I31" s="2">
         <v>30.73</v>
       </c>
       <c r="J31">
@@ -6627,7 +6630,7 @@
       <c r="H32">
         <v>0.34</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="2">
         <v>34.04</v>
       </c>
       <c r="J32">
@@ -6668,7 +6671,7 @@
       <c r="H33">
         <v>0.35</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="2">
         <v>34.6</v>
       </c>
       <c r="J33">
@@ -6709,7 +6712,7 @@
       <c r="H34">
         <v>0.38</v>
       </c>
-      <c r="I34">
+      <c r="I34" s="2">
         <v>38.450000000000003</v>
       </c>
       <c r="J34">
@@ -6750,7 +6753,7 @@
       <c r="H35">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I35">
+      <c r="I35" s="2">
         <v>27.55</v>
       </c>
       <c r="J35">
@@ -6791,7 +6794,7 @@
       <c r="H36">
         <v>0.22</v>
       </c>
-      <c r="I36">
+      <c r="I36" s="2">
         <v>22.42</v>
       </c>
       <c r="J36">
@@ -6832,7 +6835,7 @@
       <c r="H37">
         <v>0.46</v>
       </c>
-      <c r="I37">
+      <c r="I37" s="2">
         <v>46.13</v>
       </c>
       <c r="J37">
@@ -6873,7 +6876,7 @@
       <c r="H38">
         <v>0</v>
       </c>
-      <c r="I38">
+      <c r="I38" s="2">
         <v>0</v>
       </c>
       <c r="J38">
@@ -6908,7 +6911,7 @@
       <c r="H39">
         <v>0.34</v>
       </c>
-      <c r="I39">
+      <c r="I39" s="2">
         <v>34.25</v>
       </c>
       <c r="J39">
@@ -6949,7 +6952,7 @@
       <c r="H40">
         <v>0.47</v>
       </c>
-      <c r="I40">
+      <c r="I40" s="2">
         <v>46.63</v>
       </c>
       <c r="J40">
@@ -6990,7 +6993,7 @@
       <c r="H41">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I41">
+      <c r="I41" s="2">
         <v>27.88</v>
       </c>
       <c r="J41">
@@ -7031,7 +7034,7 @@
       <c r="H42">
         <v>0.33</v>
       </c>
-      <c r="I42">
+      <c r="I42" s="2">
         <v>33.15</v>
       </c>
       <c r="J42">
@@ -7072,7 +7075,7 @@
       <c r="H43">
         <v>0.31</v>
       </c>
-      <c r="I43">
+      <c r="I43" s="2">
         <v>30.64</v>
       </c>
       <c r="J43">
@@ -7113,7 +7116,7 @@
       <c r="H44">
         <v>0.38</v>
       </c>
-      <c r="I44">
+      <c r="I44" s="2">
         <v>38.17</v>
       </c>
       <c r="J44">
@@ -7154,7 +7157,7 @@
       <c r="H45">
         <v>0.38</v>
       </c>
-      <c r="I45">
+      <c r="I45" s="2">
         <v>37.590000000000003</v>
       </c>
       <c r="J45">
@@ -7195,7 +7198,7 @@
       <c r="H46">
         <v>0.24</v>
       </c>
-      <c r="I46">
+      <c r="I46" s="2">
         <v>24.27</v>
       </c>
       <c r="J46">
@@ -7236,7 +7239,7 @@
       <c r="H47">
         <v>0.34</v>
       </c>
-      <c r="I47">
+      <c r="I47" s="2">
         <v>34.32</v>
       </c>
       <c r="J47">
@@ -7277,7 +7280,7 @@
       <c r="H48">
         <v>0.35</v>
       </c>
-      <c r="I48">
+      <c r="I48" s="2">
         <v>35.08</v>
       </c>
       <c r="J48">
@@ -7318,7 +7321,7 @@
       <c r="H49">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I49">
+      <c r="I49" s="2">
         <v>29.14</v>
       </c>
       <c r="J49">
@@ -7359,7 +7362,7 @@
       <c r="H50">
         <v>0.22</v>
       </c>
-      <c r="I50">
+      <c r="I50" s="2">
         <v>22.5</v>
       </c>
       <c r="J50">
@@ -7400,7 +7403,7 @@
       <c r="H51">
         <v>0.2</v>
       </c>
-      <c r="I51">
+      <c r="I51" s="2">
         <v>20.190000000000001</v>
       </c>
       <c r="J51">
@@ -7441,7 +7444,7 @@
       <c r="H52">
         <v>0.36</v>
       </c>
-      <c r="I52">
+      <c r="I52" s="2">
         <v>35.950000000000003</v>
       </c>
       <c r="J52">
@@ -7482,7 +7485,7 @@
       <c r="H53">
         <v>0.22</v>
       </c>
-      <c r="I53">
+      <c r="I53" s="2">
         <v>21.67</v>
       </c>
       <c r="J53">
@@ -7523,7 +7526,7 @@
       <c r="H54">
         <v>0.39</v>
       </c>
-      <c r="I54">
+      <c r="I54" s="2">
         <v>39.200000000000003</v>
       </c>
       <c r="J54">
@@ -7564,7 +7567,7 @@
       <c r="H55">
         <v>0.34</v>
       </c>
-      <c r="I55">
+      <c r="I55" s="2">
         <v>34.04</v>
       </c>
       <c r="J55">
@@ -7605,7 +7608,7 @@
       <c r="H56">
         <v>0.33</v>
       </c>
-      <c r="I56">
+      <c r="I56" s="2">
         <v>32.97</v>
       </c>
       <c r="J56">
@@ -7646,7 +7649,7 @@
       <c r="H57">
         <v>0.33</v>
       </c>
-      <c r="I57">
+      <c r="I57" s="2">
         <v>32.659999999999997</v>
       </c>
       <c r="J57">
@@ -7687,7 +7690,7 @@
       <c r="H58">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I58">
+      <c r="I58" s="2">
         <v>27.91</v>
       </c>
       <c r="J58">
@@ -7728,7 +7731,7 @@
       <c r="H59">
         <v>0.23</v>
       </c>
-      <c r="I59">
+      <c r="I59" s="2">
         <v>23.09</v>
       </c>
       <c r="J59">
@@ -7769,7 +7772,7 @@
       <c r="H60">
         <v>0.39</v>
       </c>
-      <c r="I60">
+      <c r="I60" s="2">
         <v>38.51</v>
       </c>
       <c r="J60">
@@ -7810,7 +7813,7 @@
       <c r="H61">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I61">
+      <c r="I61" s="2">
         <v>27.88</v>
       </c>
       <c r="J61">
@@ -7851,7 +7854,7 @@
       <c r="H62">
         <v>0.27</v>
       </c>
-      <c r="I62">
+      <c r="I62" s="2">
         <v>26.63</v>
       </c>
       <c r="J62">
@@ -7892,7 +7895,7 @@
       <c r="H63">
         <v>0.2</v>
       </c>
-      <c r="I63">
+      <c r="I63" s="2">
         <v>19.98</v>
       </c>
       <c r="J63">
@@ -7933,7 +7936,7 @@
       <c r="H64">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I64">
+      <c r="I64" s="2">
         <v>28.34</v>
       </c>
       <c r="J64">
@@ -7974,7 +7977,7 @@
       <c r="H65">
         <v>0.34</v>
       </c>
-      <c r="I65">
+      <c r="I65" s="2">
         <v>33.659999999999997</v>
       </c>
       <c r="J65">
@@ -8015,7 +8018,7 @@
       <c r="H66">
         <v>0.2</v>
       </c>
-      <c r="I66">
+      <c r="I66" s="2">
         <v>20.25</v>
       </c>
       <c r="J66">
@@ -8056,7 +8059,7 @@
       <c r="H67">
         <v>0.2</v>
       </c>
-      <c r="I67">
+      <c r="I67" s="2">
         <v>20.27</v>
       </c>
       <c r="J67">
@@ -8097,7 +8100,7 @@
       <c r="H68">
         <v>0.2</v>
       </c>
-      <c r="I68">
+      <c r="I68" s="2">
         <v>20.39</v>
       </c>
       <c r="J68">
@@ -8138,7 +8141,7 @@
       <c r="H69">
         <v>0.37</v>
       </c>
-      <c r="I69">
+      <c r="I69" s="2">
         <v>37.49</v>
       </c>
       <c r="J69">
@@ -8179,7 +8182,7 @@
       <c r="H70">
         <v>0.31</v>
       </c>
-      <c r="I70">
+      <c r="I70" s="2">
         <v>30.97</v>
       </c>
       <c r="J70">
@@ -8220,7 +8223,7 @@
       <c r="H71">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I71">
+      <c r="I71" s="2">
         <v>29.14</v>
       </c>
       <c r="J71">
@@ -8261,7 +8264,7 @@
       <c r="H72">
         <v>0.24</v>
       </c>
-      <c r="I72">
+      <c r="I72" s="2">
         <v>23.94</v>
       </c>
       <c r="J72">
@@ -8302,7 +8305,7 @@
       <c r="H73">
         <v>0.34</v>
       </c>
-      <c r="I73">
+      <c r="I73" s="2">
         <v>34.19</v>
       </c>
       <c r="J73">
@@ -8343,7 +8346,7 @@
       <c r="H74">
         <v>0</v>
       </c>
-      <c r="I74">
+      <c r="I74" s="2">
         <v>0</v>
       </c>
       <c r="J74">
@@ -8378,7 +8381,7 @@
       <c r="H75">
         <v>0.24</v>
       </c>
-      <c r="I75">
+      <c r="I75" s="2">
         <v>23.78</v>
       </c>
       <c r="J75">
@@ -8419,7 +8422,7 @@
       <c r="H76">
         <v>0</v>
       </c>
-      <c r="I76">
+      <c r="I76" s="2">
         <v>0</v>
       </c>
       <c r="J76">
@@ -8454,7 +8457,7 @@
       <c r="H77">
         <v>0.32</v>
       </c>
-      <c r="I77">
+      <c r="I77" s="2">
         <v>32.03</v>
       </c>
       <c r="J77">
@@ -8495,7 +8498,7 @@
       <c r="H78">
         <v>0.34</v>
       </c>
-      <c r="I78">
+      <c r="I78" s="2">
         <v>33.74</v>
       </c>
       <c r="J78">
@@ -8536,7 +8539,7 @@
       <c r="H79">
         <v>0.2</v>
       </c>
-      <c r="I79">
+      <c r="I79" s="2">
         <v>20.09</v>
       </c>
       <c r="J79">
@@ -8577,7 +8580,7 @@
       <c r="H80">
         <v>0.2</v>
       </c>
-      <c r="I80">
+      <c r="I80" s="2">
         <v>20.46</v>
       </c>
       <c r="J80">
@@ -8618,7 +8621,7 @@
       <c r="H81">
         <v>0.21</v>
       </c>
-      <c r="I81">
+      <c r="I81" s="2">
         <v>21.26</v>
       </c>
       <c r="J81">
@@ -8659,7 +8662,7 @@
       <c r="H82">
         <v>0.4</v>
       </c>
-      <c r="I82">
+      <c r="I82" s="2">
         <v>40.31</v>
       </c>
       <c r="J82">
@@ -8700,7 +8703,7 @@
       <c r="H83">
         <v>0.56000000000000005</v>
       </c>
-      <c r="I83">
+      <c r="I83" s="2">
         <v>55.87</v>
       </c>
       <c r="J83">
@@ -8741,7 +8744,7 @@
       <c r="H84">
         <v>0.56000000000000005</v>
       </c>
-      <c r="I84">
+      <c r="I84" s="2">
         <v>56.34</v>
       </c>
       <c r="J84">
@@ -8782,7 +8785,7 @@
       <c r="H85">
         <v>0.41</v>
       </c>
-      <c r="I85">
+      <c r="I85" s="2">
         <v>40.840000000000003</v>
       </c>
       <c r="J85">
@@ -8823,7 +8826,7 @@
       <c r="H86">
         <v>0.27</v>
       </c>
-      <c r="I86">
+      <c r="I86" s="2">
         <v>27.4</v>
       </c>
       <c r="J86">
@@ -8864,7 +8867,7 @@
       <c r="H87">
         <v>0.23</v>
       </c>
-      <c r="I87">
+      <c r="I87" s="2">
         <v>22.67</v>
       </c>
       <c r="J87">
@@ -8905,7 +8908,7 @@
       <c r="H88">
         <v>0.34</v>
       </c>
-      <c r="I88">
+      <c r="I88" s="2">
         <v>34.49</v>
       </c>
       <c r="J88">
@@ -8946,7 +8949,7 @@
       <c r="H89">
         <v>0.41</v>
       </c>
-      <c r="I89">
+      <c r="I89" s="2">
         <v>41.05</v>
       </c>
       <c r="J89">
@@ -8987,7 +8990,7 @@
       <c r="H90">
         <v>0.3</v>
       </c>
-      <c r="I90">
+      <c r="I90" s="2">
         <v>30</v>
       </c>
       <c r="J90">
@@ -9028,7 +9031,7 @@
       <c r="H91">
         <v>0.4</v>
       </c>
-      <c r="I91">
+      <c r="I91" s="2">
         <v>39.840000000000003</v>
       </c>
       <c r="J91">
@@ -9069,7 +9072,7 @@
       <c r="H92">
         <v>0.47</v>
       </c>
-      <c r="I92">
+      <c r="I92" s="2">
         <v>46.81</v>
       </c>
       <c r="J92">
@@ -9110,7 +9113,7 @@
       <c r="H93">
         <v>0.35</v>
       </c>
-      <c r="I93">
+      <c r="I93" s="2">
         <v>35.14</v>
       </c>
       <c r="J93">
@@ -9151,7 +9154,7 @@
       <c r="H94">
         <v>0.25</v>
       </c>
-      <c r="I94">
+      <c r="I94" s="2">
         <v>24.9</v>
       </c>
       <c r="J94">
@@ -9192,7 +9195,7 @@
       <c r="H95">
         <v>0.31</v>
       </c>
-      <c r="I95">
+      <c r="I95" s="2">
         <v>31.18</v>
       </c>
       <c r="J95">
@@ -9233,7 +9236,7 @@
       <c r="H96">
         <v>0.61</v>
       </c>
-      <c r="I96">
+      <c r="I96" s="2">
         <v>61.4</v>
       </c>
       <c r="J96">
@@ -9274,7 +9277,7 @@
       <c r="H97">
         <v>0.27</v>
       </c>
-      <c r="I97">
+      <c r="I97" s="2">
         <v>26.66</v>
       </c>
       <c r="J97">
@@ -9315,7 +9318,7 @@
       <c r="H98">
         <v>0</v>
       </c>
-      <c r="I98">
+      <c r="I98" s="2">
         <v>0</v>
       </c>
       <c r="J98">
@@ -9350,7 +9353,7 @@
       <c r="H99">
         <v>0.45</v>
       </c>
-      <c r="I99">
+      <c r="I99" s="2">
         <v>45.22</v>
       </c>
       <c r="J99">
@@ -9391,7 +9394,7 @@
       <c r="H100">
         <v>0.32</v>
       </c>
-      <c r="I100">
+      <c r="I100" s="2">
         <v>32.18</v>
       </c>
       <c r="J100">
@@ -9432,7 +9435,7 @@
       <c r="H101">
         <v>0.44</v>
       </c>
-      <c r="I101">
+      <c r="I101" s="2">
         <v>44.17</v>
       </c>
       <c r="J101">
@@ -9473,7 +9476,7 @@
       <c r="H102">
         <v>0.06</v>
       </c>
-      <c r="I102">
+      <c r="I102" s="2">
         <v>5.6</v>
       </c>
       <c r="J102">
@@ -9514,7 +9517,7 @@
       <c r="H103">
         <v>0.33</v>
       </c>
-      <c r="I103">
+      <c r="I103" s="2">
         <v>32.96</v>
       </c>
       <c r="J103">
@@ -9555,7 +9558,7 @@
       <c r="H104">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I104">
+      <c r="I104" s="2">
         <v>27.86</v>
       </c>
       <c r="J104">
@@ -9596,7 +9599,7 @@
       <c r="H105">
         <v>0.33</v>
       </c>
-      <c r="I105">
+      <c r="I105" s="2">
         <v>33.01</v>
       </c>
       <c r="J105">
@@ -9637,7 +9640,7 @@
       <c r="H106">
         <v>0.42</v>
       </c>
-      <c r="I106">
+      <c r="I106" s="2">
         <v>42.41</v>
       </c>
       <c r="J106">
@@ -9678,7 +9681,7 @@
       <c r="H107">
         <v>0.24</v>
       </c>
-      <c r="I107">
+      <c r="I107" s="2">
         <v>24.06</v>
       </c>
       <c r="J107">
@@ -9719,7 +9722,7 @@
       <c r="H108">
         <v>0.34</v>
       </c>
-      <c r="I108">
+      <c r="I108" s="2">
         <v>34.42</v>
       </c>
       <c r="J108">
@@ -9760,7 +9763,7 @@
       <c r="H109">
         <v>0.3</v>
       </c>
-      <c r="I109">
+      <c r="I109" s="2">
         <v>30.48</v>
       </c>
       <c r="J109">
@@ -9801,7 +9804,7 @@
       <c r="H110">
         <v>0.25</v>
       </c>
-      <c r="I110">
+      <c r="I110" s="2">
         <v>25.25</v>
       </c>
       <c r="J110">
@@ -9842,7 +9845,7 @@
       <c r="H111">
         <v>0.38</v>
       </c>
-      <c r="I111">
+      <c r="I111" s="2">
         <v>38.19</v>
       </c>
       <c r="J111">
@@ -9883,7 +9886,7 @@
       <c r="H112">
         <v>0.35</v>
       </c>
-      <c r="I112">
+      <c r="I112" s="2">
         <v>34.71</v>
       </c>
       <c r="J112">
@@ -9924,7 +9927,7 @@
       <c r="H113">
         <v>0.34</v>
       </c>
-      <c r="I113">
+      <c r="I113" s="2">
         <v>33.54</v>
       </c>
       <c r="J113">
@@ -9965,7 +9968,7 @@
       <c r="H114">
         <v>0.33</v>
       </c>
-      <c r="I114">
+      <c r="I114" s="2">
         <v>32.56</v>
       </c>
       <c r="J114">
@@ -10006,7 +10009,7 @@
       <c r="H115">
         <v>0.35</v>
       </c>
-      <c r="I115">
+      <c r="I115" s="2">
         <v>34.75</v>
       </c>
       <c r="J115">
@@ -10047,7 +10050,7 @@
       <c r="H116">
         <v>0.25</v>
       </c>
-      <c r="I116">
+      <c r="I116" s="2">
         <v>24.88</v>
       </c>
       <c r="J116">
@@ -10088,7 +10091,7 @@
       <c r="H117">
         <v>0.39</v>
       </c>
-      <c r="I117">
+      <c r="I117" s="2">
         <v>38.979999999999997</v>
       </c>
       <c r="J117">
@@ -10129,7 +10132,7 @@
       <c r="H118">
         <v>0</v>
       </c>
-      <c r="I118">
+      <c r="I118" s="2">
         <v>0</v>
       </c>
       <c r="J118">
@@ -10164,7 +10167,7 @@
       <c r="H119">
         <v>0.36</v>
       </c>
-      <c r="I119">
+      <c r="I119" s="2">
         <v>36.49</v>
       </c>
       <c r="J119">
@@ -10205,7 +10208,7 @@
       <c r="H120">
         <v>0.37</v>
       </c>
-      <c r="I120">
+      <c r="I120" s="2">
         <v>37.04</v>
       </c>
       <c r="J120">
@@ -10246,7 +10249,7 @@
       <c r="H121">
         <v>0.39</v>
       </c>
-      <c r="I121">
+      <c r="I121" s="2">
         <v>39.450000000000003</v>
       </c>
       <c r="J121">
@@ -10287,7 +10290,7 @@
       <c r="H122">
         <v>0.36</v>
       </c>
-      <c r="I122">
+      <c r="I122" s="2">
         <v>35.93</v>
       </c>
       <c r="J122">
@@ -10328,7 +10331,7 @@
       <c r="H123">
         <v>0.36</v>
       </c>
-      <c r="I123">
+      <c r="I123" s="2">
         <v>35.92</v>
       </c>
       <c r="J123">
@@ -10369,7 +10372,7 @@
       <c r="H124">
         <v>0.37</v>
       </c>
-      <c r="I124">
+      <c r="I124" s="2">
         <v>36.56</v>
       </c>
       <c r="J124">
@@ -10410,7 +10413,7 @@
       <c r="H125">
         <v>0</v>
       </c>
-      <c r="I125">
+      <c r="I125" s="2">
         <v>0</v>
       </c>
       <c r="J125">
@@ -10445,7 +10448,7 @@
       <c r="H126">
         <v>0.25</v>
       </c>
-      <c r="I126">
+      <c r="I126" s="2">
         <v>25.04</v>
       </c>
       <c r="J126">
@@ -10486,7 +10489,7 @@
       <c r="H127">
         <v>0.33</v>
       </c>
-      <c r="I127">
+      <c r="I127" s="2">
         <v>32.86</v>
       </c>
       <c r="J127">
@@ -10527,7 +10530,7 @@
       <c r="H128">
         <v>0.25</v>
       </c>
-      <c r="I128">
+      <c r="I128" s="2">
         <v>24.61</v>
       </c>
       <c r="J128">
@@ -10568,7 +10571,7 @@
       <c r="H129">
         <v>0.37</v>
       </c>
-      <c r="I129">
+      <c r="I129" s="2">
         <v>37.04</v>
       </c>
       <c r="J129">
@@ -10609,7 +10612,7 @@
       <c r="H130">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I130">
+      <c r="I130" s="2">
         <v>29.03</v>
       </c>
       <c r="J130">
@@ -10650,7 +10653,7 @@
       <c r="H131">
         <v>0.4</v>
       </c>
-      <c r="I131">
+      <c r="I131" s="2">
         <v>39.659999999999997</v>
       </c>
       <c r="J131">
@@ -10691,7 +10694,7 @@
       <c r="H132">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I132">
+      <c r="I132" s="2">
         <v>28.26</v>
       </c>
       <c r="J132">
@@ -10732,7 +10735,7 @@
       <c r="H133">
         <v>0.33</v>
       </c>
-      <c r="I133">
+      <c r="I133" s="2">
         <v>33.28</v>
       </c>
       <c r="J133">
@@ -10773,7 +10776,7 @@
       <c r="H134">
         <v>0.34</v>
       </c>
-      <c r="I134">
+      <c r="I134" s="2">
         <v>33.659999999999997</v>
       </c>
       <c r="J134">
@@ -10814,7 +10817,7 @@
       <c r="H135">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I135">
+      <c r="I135" s="2">
         <v>28.41</v>
       </c>
       <c r="J135">
@@ -10855,7 +10858,7 @@
       <c r="H136">
         <v>0.27</v>
       </c>
-      <c r="I136">
+      <c r="I136" s="2">
         <v>26.61</v>
       </c>
       <c r="J136">
@@ -10896,7 +10899,7 @@
       <c r="H137">
         <v>0.32</v>
       </c>
-      <c r="I137">
+      <c r="I137" s="2">
         <v>32.11</v>
       </c>
       <c r="J137">
@@ -10937,7 +10940,7 @@
       <c r="H138">
         <v>0.41</v>
       </c>
-      <c r="I138">
+      <c r="I138" s="2">
         <v>40.909999999999997</v>
       </c>
       <c r="J138">
@@ -10978,7 +10981,7 @@
       <c r="H139">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I139">
+      <c r="I139" s="2">
         <v>27.67</v>
       </c>
       <c r="J139">
@@ -11019,7 +11022,7 @@
       <c r="H140">
         <v>0.25</v>
       </c>
-      <c r="I140">
+      <c r="I140" s="2">
         <v>25.11</v>
       </c>
       <c r="J140">
@@ -11060,7 +11063,7 @@
       <c r="H141">
         <v>0.27</v>
       </c>
-      <c r="I141">
+      <c r="I141" s="2">
         <v>26.94</v>
       </c>
       <c r="J141">
@@ -11101,7 +11104,7 @@
       <c r="H142">
         <v>0.22</v>
       </c>
-      <c r="I142">
+      <c r="I142" s="2">
         <v>22.27</v>
       </c>
       <c r="J142">
@@ -11142,7 +11145,7 @@
       <c r="H143">
         <v>0.41</v>
       </c>
-      <c r="I143">
+      <c r="I143" s="2">
         <v>41.03</v>
       </c>
       <c r="J143">
@@ -11183,7 +11186,7 @@
       <c r="H144">
         <v>0.21</v>
       </c>
-      <c r="I144">
+      <c r="I144" s="2">
         <v>21.25</v>
       </c>
       <c r="J144">
@@ -11224,7 +11227,7 @@
       <c r="H145">
         <v>0.23</v>
       </c>
-      <c r="I145">
+      <c r="I145" s="2">
         <v>23.22</v>
       </c>
       <c r="J145">
@@ -11265,7 +11268,7 @@
       <c r="H146">
         <v>0.27</v>
       </c>
-      <c r="I146">
+      <c r="I146" s="2">
         <v>26.58</v>
       </c>
       <c r="J146">
@@ -11306,7 +11309,7 @@
       <c r="H147">
         <v>0.3</v>
       </c>
-      <c r="I147">
+      <c r="I147" s="2">
         <v>30.36</v>
       </c>
       <c r="J147">
@@ -11347,7 +11350,7 @@
       <c r="H148">
         <v>0.27</v>
       </c>
-      <c r="I148">
+      <c r="I148" s="2">
         <v>27.42</v>
       </c>
       <c r="J148">
@@ -11388,7 +11391,7 @@
       <c r="H149">
         <v>0.26</v>
       </c>
-      <c r="I149">
+      <c r="I149" s="2">
         <v>26.34</v>
       </c>
       <c r="J149">
@@ -11429,7 +11432,7 @@
       <c r="H150">
         <v>0</v>
       </c>
-      <c r="I150">
+      <c r="I150" s="2">
         <v>0</v>
       </c>
       <c r="J150">
@@ -11464,7 +11467,7 @@
       <c r="H151">
         <v>0.33</v>
       </c>
-      <c r="I151">
+      <c r="I151" s="2">
         <v>32.619999999999997</v>
       </c>
       <c r="J151">
@@ -11505,7 +11508,7 @@
       <c r="H152">
         <v>0.34</v>
       </c>
-      <c r="I152">
+      <c r="I152" s="2">
         <v>34.11</v>
       </c>
       <c r="J152">
@@ -11546,7 +11549,7 @@
       <c r="H153">
         <v>0.43</v>
       </c>
-      <c r="I153">
+      <c r="I153" s="2">
         <v>42.93</v>
       </c>
       <c r="J153">
@@ -11587,7 +11590,7 @@
       <c r="H154">
         <v>0.3</v>
       </c>
-      <c r="I154">
+      <c r="I154" s="2">
         <v>29.62</v>
       </c>
       <c r="J154">
@@ -11628,7 +11631,7 @@
       <c r="H155">
         <v>0.35</v>
       </c>
-      <c r="I155">
+      <c r="I155" s="2">
         <v>34.799999999999997</v>
       </c>
       <c r="J155">
@@ -11669,7 +11672,7 @@
       <c r="H156">
         <v>0.36</v>
       </c>
-      <c r="I156">
+      <c r="I156" s="2">
         <v>35.86</v>
       </c>
       <c r="J156">
@@ -11710,7 +11713,7 @@
       <c r="H157">
         <v>0.31</v>
       </c>
-      <c r="I157">
+      <c r="I157" s="2">
         <v>30.79</v>
       </c>
       <c r="J157">
@@ -11751,7 +11754,7 @@
       <c r="H158">
         <v>0.32</v>
       </c>
-      <c r="I158">
+      <c r="I158" s="2">
         <v>32.340000000000003</v>
       </c>
       <c r="J158">
@@ -11792,7 +11795,7 @@
       <c r="H159">
         <v>0.34</v>
       </c>
-      <c r="I159">
+      <c r="I159" s="2">
         <v>34.11</v>
       </c>
       <c r="J159">
@@ -11833,7 +11836,7 @@
       <c r="H160">
         <v>0.23</v>
       </c>
-      <c r="I160">
+      <c r="I160" s="2">
         <v>23.01</v>
       </c>
       <c r="J160">
@@ -11874,7 +11877,7 @@
       <c r="H161">
         <v>0.33</v>
       </c>
-      <c r="I161">
+      <c r="I161" s="2">
         <v>33.5</v>
       </c>
       <c r="J161">
@@ -11915,7 +11918,7 @@
       <c r="H162">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I162">
+      <c r="I162" s="2">
         <v>28.32</v>
       </c>
       <c r="J162">
@@ -11956,7 +11959,7 @@
       <c r="H163">
         <v>0.34</v>
       </c>
-      <c r="I163">
+      <c r="I163" s="2">
         <v>34.15</v>
       </c>
       <c r="J163">
@@ -11997,7 +12000,7 @@
       <c r="H164">
         <v>0.16</v>
       </c>
-      <c r="I164">
+      <c r="I164" s="2">
         <v>15.83</v>
       </c>
       <c r="J164">
@@ -12038,7 +12041,7 @@
       <c r="H165">
         <v>0.25</v>
       </c>
-      <c r="I165">
+      <c r="I165" s="2">
         <v>25.37</v>
       </c>
       <c r="J165">
@@ -12079,7 +12082,7 @@
       <c r="H166">
         <v>0.25</v>
       </c>
-      <c r="I166">
+      <c r="I166" s="2">
         <v>25.23</v>
       </c>
       <c r="J166">
@@ -12120,7 +12123,7 @@
       <c r="H167">
         <v>0.33</v>
       </c>
-      <c r="I167">
+      <c r="I167" s="2">
         <v>33.21</v>
       </c>
       <c r="J167">
@@ -12161,7 +12164,7 @@
       <c r="H168">
         <v>0.37</v>
       </c>
-      <c r="I168">
+      <c r="I168" s="2">
         <v>36.6</v>
       </c>
       <c r="J168">
@@ -12202,7 +12205,7 @@
       <c r="H169">
         <v>0.23</v>
       </c>
-      <c r="I169">
+      <c r="I169" s="2">
         <v>23.18</v>
       </c>
       <c r="J169">
@@ -12243,7 +12246,7 @@
       <c r="H170">
         <v>0.26</v>
       </c>
-      <c r="I170">
+      <c r="I170" s="2">
         <v>26.48</v>
       </c>
       <c r="J170">
@@ -12284,7 +12287,7 @@
       <c r="H171">
         <v>0</v>
       </c>
-      <c r="I171">
+      <c r="I171" s="2">
         <v>0</v>
       </c>
       <c r="J171">
@@ -12319,7 +12322,7 @@
       <c r="H172">
         <v>0.35</v>
       </c>
-      <c r="I172">
+      <c r="I172" s="2">
         <v>35.119999999999997</v>
       </c>
       <c r="J172">
@@ -12360,7 +12363,7 @@
       <c r="H173">
         <v>0.36</v>
       </c>
-      <c r="I173">
+      <c r="I173" s="2">
         <v>35.58</v>
       </c>
       <c r="J173">
@@ -12401,7 +12404,7 @@
       <c r="H174">
         <v>0.35</v>
       </c>
-      <c r="I174">
+      <c r="I174" s="2">
         <v>35.15</v>
       </c>
       <c r="J174">
@@ -12442,7 +12445,7 @@
       <c r="H175">
         <v>0.43</v>
       </c>
-      <c r="I175">
+      <c r="I175" s="2">
         <v>43.03</v>
       </c>
       <c r="J175">
@@ -12483,7 +12486,7 @@
       <c r="H176">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I176">
+      <c r="I176" s="2">
         <v>27.98</v>
       </c>
       <c r="J176">
@@ -12524,7 +12527,7 @@
       <c r="H177">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I177">
+      <c r="I177" s="2">
         <v>28.12</v>
       </c>
       <c r="J177">
@@ -12565,7 +12568,7 @@
       <c r="H178">
         <v>0.34</v>
       </c>
-      <c r="I178">
+      <c r="I178" s="2">
         <v>34.42</v>
       </c>
       <c r="J178">
@@ -12606,7 +12609,7 @@
       <c r="H179">
         <v>0.3</v>
       </c>
-      <c r="I179">
+      <c r="I179" s="2">
         <v>29.93</v>
       </c>
       <c r="J179">
@@ -12647,7 +12650,7 @@
       <c r="H180">
         <v>0.31</v>
       </c>
-      <c r="I180">
+      <c r="I180" s="2">
         <v>30.55</v>
       </c>
       <c r="J180">
@@ -12688,7 +12691,7 @@
       <c r="H181">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I181">
+      <c r="I181" s="2">
         <v>28.4</v>
       </c>
       <c r="J181">
@@ -12729,7 +12732,7 @@
       <c r="H182">
         <v>0.24</v>
       </c>
-      <c r="I182">
+      <c r="I182" s="2">
         <v>23.94</v>
       </c>
       <c r="J182">
@@ -12770,7 +12773,7 @@
       <c r="H183">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I183">
+      <c r="I183" s="2">
         <v>27.96</v>
       </c>
       <c r="J183">
@@ -12811,7 +12814,7 @@
       <c r="H184">
         <v>0.34</v>
       </c>
-      <c r="I184">
+      <c r="I184" s="2">
         <v>34.119999999999997</v>
       </c>
       <c r="J184">
@@ -12852,7 +12855,7 @@
       <c r="H185">
         <v>0.25</v>
       </c>
-      <c r="I185">
+      <c r="I185" s="2">
         <v>25.05</v>
       </c>
       <c r="J185">
@@ -12893,7 +12896,7 @@
       <c r="H186">
         <v>0.25</v>
       </c>
-      <c r="I186">
+      <c r="I186" s="2">
         <v>24.61</v>
       </c>
       <c r="J186">
@@ -12934,7 +12937,7 @@
       <c r="H187">
         <v>0.31</v>
       </c>
-      <c r="I187">
+      <c r="I187" s="2">
         <v>30.58</v>
       </c>
       <c r="J187">
@@ -12975,7 +12978,7 @@
       <c r="H188">
         <v>0.31</v>
       </c>
-      <c r="I188">
+      <c r="I188" s="2">
         <v>31.49</v>
       </c>
       <c r="J188">
@@ -13016,7 +13019,7 @@
       <c r="H189">
         <v>0.32</v>
       </c>
-      <c r="I189">
+      <c r="I189" s="2">
         <v>31.92</v>
       </c>
       <c r="J189">
@@ -13057,7 +13060,7 @@
       <c r="H190">
         <v>0.32</v>
       </c>
-      <c r="I190">
+      <c r="I190" s="2">
         <v>31.77</v>
       </c>
       <c r="J190">
@@ -13098,7 +13101,7 @@
       <c r="H191">
         <v>0</v>
       </c>
-      <c r="I191">
+      <c r="I191" s="2">
         <v>0</v>
       </c>
       <c r="J191">
@@ -13133,7 +13136,7 @@
       <c r="H192">
         <v>0.25</v>
       </c>
-      <c r="I192">
+      <c r="I192" s="2">
         <v>25.5</v>
       </c>
       <c r="J192">
@@ -13174,7 +13177,7 @@
       <c r="H193">
         <v>0.24</v>
       </c>
-      <c r="I193">
+      <c r="I193" s="2">
         <v>23.97</v>
       </c>
       <c r="J193">
@@ -13215,7 +13218,7 @@
       <c r="H194">
         <v>0.24</v>
       </c>
-      <c r="I194">
+      <c r="I194" s="2">
         <v>24.14</v>
       </c>
       <c r="J194">
@@ -13256,7 +13259,7 @@
       <c r="H195">
         <v>0.19</v>
       </c>
-      <c r="I195">
+      <c r="I195" s="2">
         <v>19.48</v>
       </c>
       <c r="J195">
@@ -13297,7 +13300,7 @@
       <c r="H196">
         <v>0.21</v>
       </c>
-      <c r="I196">
+      <c r="I196" s="2">
         <v>20.57</v>
       </c>
       <c r="J196">
@@ -13338,7 +13341,7 @@
       <c r="H197">
         <v>0.22</v>
       </c>
-      <c r="I197">
+      <c r="I197" s="2">
         <v>21.54</v>
       </c>
       <c r="J197">
@@ -13379,7 +13382,7 @@
       <c r="H198">
         <v>0.3</v>
       </c>
-      <c r="I198">
+      <c r="I198" s="2">
         <v>30.07</v>
       </c>
       <c r="J198">
@@ -13420,7 +13423,7 @@
       <c r="H199">
         <v>0.27</v>
       </c>
-      <c r="I199">
+      <c r="I199" s="2">
         <v>26.8</v>
       </c>
       <c r="J199">
@@ -13461,7 +13464,7 @@
       <c r="H200">
         <v>0.23</v>
       </c>
-      <c r="I200">
+      <c r="I200" s="2">
         <v>22.83</v>
       </c>
       <c r="J200">
@@ -13502,7 +13505,7 @@
       <c r="H201">
         <v>0.25</v>
       </c>
-      <c r="I201">
+      <c r="I201" s="2">
         <v>25.33</v>
       </c>
       <c r="J201">
@@ -13543,7 +13546,7 @@
       <c r="H202">
         <v>0.24</v>
       </c>
-      <c r="I202">
+      <c r="I202" s="2">
         <v>23.57</v>
       </c>
       <c r="J202">
@@ -13584,7 +13587,7 @@
       <c r="H203">
         <v>0.33</v>
       </c>
-      <c r="I203">
+      <c r="I203" s="2">
         <v>33.06</v>
       </c>
       <c r="J203">
@@ -13625,7 +13628,7 @@
       <c r="H204">
         <v>0.22</v>
       </c>
-      <c r="I204">
+      <c r="I204" s="2">
         <v>22.16</v>
       </c>
       <c r="J204">
@@ -13666,7 +13669,7 @@
       <c r="H205">
         <v>0.36</v>
       </c>
-      <c r="I205">
+      <c r="I205" s="2">
         <v>35.76</v>
       </c>
       <c r="J205">
@@ -13707,7 +13710,7 @@
       <c r="H206">
         <v>0.31</v>
       </c>
-      <c r="I206">
+      <c r="I206" s="2">
         <v>30.84</v>
       </c>
       <c r="J206">
@@ -13748,7 +13751,7 @@
       <c r="H207">
         <v>0.23</v>
       </c>
-      <c r="I207">
+      <c r="I207" s="2">
         <v>22.55</v>
       </c>
       <c r="J207">
@@ -13789,7 +13792,7 @@
       <c r="H208">
         <v>0.37</v>
       </c>
-      <c r="I208">
+      <c r="I208" s="2">
         <v>36.99</v>
       </c>
       <c r="J208">
@@ -13830,7 +13833,7 @@
       <c r="H209">
         <v>0.44</v>
       </c>
-      <c r="I209">
+      <c r="I209" s="2">
         <v>44.38</v>
       </c>
       <c r="J209">
@@ -13871,7 +13874,7 @@
       <c r="H210">
         <v>0.26</v>
       </c>
-      <c r="I210">
+      <c r="I210" s="2">
         <v>26.33</v>
       </c>
       <c r="J210">
@@ -13912,7 +13915,7 @@
       <c r="H211">
         <v>0.39</v>
       </c>
-      <c r="I211">
+      <c r="I211" s="2">
         <v>38.64</v>
       </c>
       <c r="J211">
@@ -13953,7 +13956,7 @@
       <c r="H212">
         <v>0.3</v>
       </c>
-      <c r="I212">
+      <c r="I212" s="2">
         <v>30.21</v>
       </c>
       <c r="J212">
@@ -13994,7 +13997,7 @@
       <c r="H213">
         <v>0.25</v>
       </c>
-      <c r="I213">
+      <c r="I213" s="2">
         <v>24.72</v>
       </c>
       <c r="J213">
@@ -14035,7 +14038,7 @@
       <c r="H214">
         <v>0.31</v>
       </c>
-      <c r="I214">
+      <c r="I214" s="2">
         <v>31.48</v>
       </c>
       <c r="J214">
@@ -14076,7 +14079,7 @@
       <c r="H215">
         <v>0.48</v>
       </c>
-      <c r="I215">
+      <c r="I215" s="2">
         <v>47.61</v>
       </c>
       <c r="J215">
@@ -14117,7 +14120,7 @@
       <c r="H216">
         <v>0.61</v>
       </c>
-      <c r="I216">
+      <c r="I216" s="2">
         <v>61.4</v>
       </c>
       <c r="J216">
@@ -14158,7 +14161,7 @@
       <c r="H217">
         <v>0.5</v>
       </c>
-      <c r="I217">
+      <c r="I217" s="2">
         <v>50.2</v>
       </c>
       <c r="J217">
@@ -14199,7 +14202,7 @@
       <c r="H218">
         <v>0.23</v>
       </c>
-      <c r="I218">
+      <c r="I218" s="2">
         <v>22.59</v>
       </c>
       <c r="J218">
@@ -14240,7 +14243,7 @@
       <c r="H219">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I219">
+      <c r="I219" s="2">
         <v>29.17</v>
       </c>
       <c r="J219">
@@ -14281,7 +14284,7 @@
       <c r="H220">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I220">
+      <c r="I220" s="2">
         <v>14.04</v>
       </c>
       <c r="J220">
@@ -14322,7 +14325,7 @@
       <c r="H221">
         <v>0.49</v>
       </c>
-      <c r="I221">
+      <c r="I221" s="2">
         <v>49.35</v>
       </c>
       <c r="J221">
@@ -14363,7 +14366,7 @@
       <c r="H222">
         <v>0.15</v>
       </c>
-      <c r="I222">
+      <c r="I222" s="2">
         <v>15.46</v>
       </c>
       <c r="J222">
@@ -14404,7 +14407,7 @@
       <c r="H223">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I223">
+      <c r="I223" s="2">
         <v>27.9</v>
       </c>
       <c r="J223">
@@ -14445,7 +14448,7 @@
       <c r="H224">
         <v>0.26</v>
       </c>
-      <c r="I224">
+      <c r="I224" s="2">
         <v>26.15</v>
       </c>
       <c r="J224">
@@ -14486,7 +14489,7 @@
       <c r="H225">
         <v>0.2</v>
       </c>
-      <c r="I225">
+      <c r="I225" s="2">
         <v>20.25</v>
       </c>
       <c r="J225">
@@ -14527,7 +14530,7 @@
       <c r="H226">
         <v>0.32</v>
       </c>
-      <c r="I226">
+      <c r="I226" s="2">
         <v>32.229999999999997</v>
       </c>
       <c r="J226">
@@ -14568,7 +14571,7 @@
       <c r="H227">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I227">
+      <c r="I227" s="2">
         <v>27.56</v>
       </c>
       <c r="J227">
@@ -14609,7 +14612,7 @@
       <c r="H228">
         <v>0.19</v>
       </c>
-      <c r="I228">
+      <c r="I228" s="2">
         <v>18.670000000000002</v>
       </c>
       <c r="J228">
@@ -14650,7 +14653,7 @@
       <c r="H229">
         <v>0</v>
       </c>
-      <c r="I229">
+      <c r="I229" s="2">
         <v>0</v>
       </c>
       <c r="J229">
@@ -14685,7 +14688,7 @@
       <c r="H230">
         <v>0.25</v>
       </c>
-      <c r="I230">
+      <c r="I230" s="2">
         <v>24.85</v>
       </c>
       <c r="J230">
@@ -14726,7 +14729,7 @@
       <c r="H231">
         <v>0.4</v>
       </c>
-      <c r="I231">
+      <c r="I231" s="2">
         <v>40.18</v>
       </c>
       <c r="J231">
@@ -14767,7 +14770,7 @@
       <c r="H232">
         <v>0.32</v>
       </c>
-      <c r="I232">
+      <c r="I232" s="2">
         <v>31.63</v>
       </c>
       <c r="J232">
@@ -14808,7 +14811,7 @@
       <c r="H233">
         <v>0</v>
       </c>
-      <c r="I233">
+      <c r="I233" s="2">
         <v>0</v>
       </c>
       <c r="J233">
@@ -14843,7 +14846,7 @@
       <c r="H234">
         <v>0.24</v>
       </c>
-      <c r="I234">
+      <c r="I234" s="2">
         <v>24.41</v>
       </c>
       <c r="J234">
@@ -14884,7 +14887,7 @@
       <c r="H235">
         <v>0.26</v>
       </c>
-      <c r="I235">
+      <c r="I235" s="2">
         <v>26.19</v>
       </c>
       <c r="J235">
@@ -14925,7 +14928,7 @@
       <c r="H236">
         <v>0.33</v>
       </c>
-      <c r="I236">
+      <c r="I236" s="2">
         <v>32.81</v>
       </c>
       <c r="J236">
@@ -14966,7 +14969,7 @@
       <c r="H237">
         <v>0.35</v>
       </c>
-      <c r="I237">
+      <c r="I237" s="2">
         <v>34.979999999999997</v>
       </c>
       <c r="J237">
@@ -15007,7 +15010,7 @@
       <c r="H238">
         <v>0.37</v>
       </c>
-      <c r="I238">
+      <c r="I238" s="2">
         <v>36.729999999999997</v>
       </c>
       <c r="J238">
@@ -15048,7 +15051,7 @@
       <c r="H239">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I239">
+      <c r="I239" s="2">
         <v>28.6</v>
       </c>
       <c r="J239">
@@ -15089,7 +15092,7 @@
       <c r="H240">
         <v>0.35</v>
       </c>
-      <c r="I240">
+      <c r="I240" s="2">
         <v>35.119999999999997</v>
       </c>
       <c r="J240">
@@ -15130,7 +15133,7 @@
       <c r="H241">
         <v>0.37</v>
       </c>
-      <c r="I241">
+      <c r="I241" s="2">
         <v>36.99</v>
       </c>
       <c r="J241">
@@ -15171,7 +15174,7 @@
       <c r="H242">
         <v>0.26</v>
       </c>
-      <c r="I242">
+      <c r="I242" s="2">
         <v>26.14</v>
       </c>
       <c r="J242">
@@ -15212,7 +15215,7 @@
       <c r="H243">
         <v>0.36</v>
       </c>
-      <c r="I243">
+      <c r="I243" s="2">
         <v>36.18</v>
       </c>
       <c r="J243">
@@ -15253,7 +15256,7 @@
       <c r="H244">
         <v>0.3</v>
       </c>
-      <c r="I244">
+      <c r="I244" s="2">
         <v>29.78</v>
       </c>
       <c r="J244">
@@ -15294,7 +15297,7 @@
       <c r="H245">
         <v>0.27</v>
       </c>
-      <c r="I245">
+      <c r="I245" s="2">
         <v>27.07</v>
       </c>
       <c r="J245">
@@ -15335,7 +15338,7 @@
       <c r="H246">
         <v>0.36</v>
       </c>
-      <c r="I246">
+      <c r="I246" s="2">
         <v>35.83</v>
       </c>
       <c r="J246">
@@ -15376,7 +15379,7 @@
       <c r="H247">
         <v>0.27</v>
       </c>
-      <c r="I247">
+      <c r="I247" s="2">
         <v>27.3</v>
       </c>
       <c r="J247">
@@ -15417,7 +15420,7 @@
       <c r="H248">
         <v>0.27</v>
       </c>
-      <c r="I248">
+      <c r="I248" s="2">
         <v>27.12</v>
       </c>
       <c r="J248">
@@ -15458,7 +15461,7 @@
       <c r="H249">
         <v>0.22</v>
       </c>
-      <c r="I249">
+      <c r="I249" s="2">
         <v>22.22</v>
       </c>
       <c r="J249">
@@ -15499,7 +15502,7 @@
       <c r="H250">
         <v>0.35</v>
       </c>
-      <c r="I250">
+      <c r="I250" s="2">
         <v>34.83</v>
       </c>
       <c r="J250">
@@ -15540,7 +15543,7 @@
       <c r="H251">
         <v>0.16</v>
       </c>
-      <c r="I251">
+      <c r="I251" s="2">
         <v>16.29</v>
       </c>
       <c r="J251">
@@ -15581,7 +15584,7 @@
       <c r="H252">
         <v>0.43</v>
       </c>
-      <c r="I252">
+      <c r="I252" s="2">
         <v>42.58</v>
       </c>
       <c r="J252">
@@ -15622,7 +15625,7 @@
       <c r="H253">
         <v>0.31</v>
       </c>
-      <c r="I253">
+      <c r="I253" s="2">
         <v>30.98</v>
       </c>
       <c r="J253">
@@ -15663,7 +15666,7 @@
       <c r="H254">
         <v>0.36</v>
       </c>
-      <c r="I254">
+      <c r="I254" s="2">
         <v>35.54</v>
       </c>
       <c r="J254">
@@ -15704,7 +15707,7 @@
       <c r="H255">
         <v>0.27</v>
       </c>
-      <c r="I255">
+      <c r="I255" s="2">
         <v>27.13</v>
       </c>
       <c r="J255">
@@ -15745,7 +15748,7 @@
       <c r="H256">
         <v>0.36</v>
       </c>
-      <c r="I256">
+      <c r="I256" s="2">
         <v>35.93</v>
       </c>
       <c r="J256">
@@ -15786,7 +15789,7 @@
       <c r="H257">
         <v>0.35</v>
       </c>
-      <c r="I257">
+      <c r="I257" s="2">
         <v>34.520000000000003</v>
       </c>
       <c r="J257">
@@ -15827,7 +15830,7 @@
       <c r="H258">
         <v>0.16</v>
       </c>
-      <c r="I258">
+      <c r="I258" s="2">
         <v>15.57</v>
       </c>
       <c r="J258">
@@ -15868,7 +15871,7 @@
       <c r="H259">
         <v>0.3</v>
       </c>
-      <c r="I259">
+      <c r="I259" s="2">
         <v>29.74</v>
       </c>
       <c r="J259">
@@ -15909,7 +15912,7 @@
       <c r="H260">
         <v>0.34</v>
       </c>
-      <c r="I260">
+      <c r="I260" s="2">
         <v>34.479999999999997</v>
       </c>
       <c r="J260">
@@ -15950,7 +15953,7 @@
       <c r="H261">
         <v>0.41</v>
       </c>
-      <c r="I261">
+      <c r="I261" s="2">
         <v>41.28</v>
       </c>
       <c r="J261">
@@ -15991,7 +15994,7 @@
       <c r="H262">
         <v>0.3</v>
       </c>
-      <c r="I262">
+      <c r="I262" s="2">
         <v>29.68</v>
       </c>
       <c r="J262">
@@ -16032,7 +16035,7 @@
       <c r="H263">
         <v>0.37</v>
       </c>
-      <c r="I263">
+      <c r="I263" s="2">
         <v>36.74</v>
       </c>
       <c r="J263">
@@ -16073,7 +16076,7 @@
       <c r="H264">
         <v>0.27</v>
       </c>
-      <c r="I264">
+      <c r="I264" s="2">
         <v>26.86</v>
       </c>
       <c r="J264">
@@ -16114,7 +16117,7 @@
       <c r="H265">
         <v>0.31</v>
       </c>
-      <c r="I265">
+      <c r="I265" s="2">
         <v>30.63</v>
       </c>
       <c r="J265">
@@ -16155,7 +16158,7 @@
       <c r="H266">
         <v>0.26</v>
       </c>
-      <c r="I266">
+      <c r="I266" s="2">
         <v>26.16</v>
       </c>
       <c r="J266">
@@ -16196,7 +16199,7 @@
       <c r="H267">
         <v>0.33</v>
       </c>
-      <c r="I267">
+      <c r="I267" s="2">
         <v>32.65</v>
       </c>
       <c r="J267">
@@ -16237,7 +16240,7 @@
       <c r="H268">
         <v>0.39</v>
       </c>
-      <c r="I268">
+      <c r="I268" s="2">
         <v>38.659999999999997</v>
       </c>
       <c r="J268">
@@ -16278,7 +16281,7 @@
       <c r="H269">
         <v>0.42</v>
       </c>
-      <c r="I269">
+      <c r="I269" s="2">
         <v>41.73</v>
       </c>
       <c r="J269">
@@ -16319,7 +16322,7 @@
       <c r="H270">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I270">
+      <c r="I270" s="2">
         <v>29.18</v>
       </c>
       <c r="J270">
@@ -16360,7 +16363,7 @@
       <c r="H271">
         <v>0.31</v>
       </c>
-      <c r="I271">
+      <c r="I271" s="2">
         <v>30.84</v>
       </c>
       <c r="J271">
@@ -16401,7 +16404,7 @@
       <c r="H272">
         <v>0.46</v>
       </c>
-      <c r="I272">
+      <c r="I272" s="2">
         <v>45.85</v>
       </c>
       <c r="J272">
@@ -16442,7 +16445,7 @@
       <c r="H273">
         <v>0.25</v>
       </c>
-      <c r="I273">
+      <c r="I273" s="2">
         <v>25.34</v>
       </c>
       <c r="J273">
@@ -16483,7 +16486,7 @@
       <c r="H274">
         <v>0.4</v>
       </c>
-      <c r="I274">
+      <c r="I274" s="2">
         <v>40.25</v>
       </c>
       <c r="J274">
@@ -16524,7 +16527,7 @@
       <c r="H275">
         <v>0.33</v>
       </c>
-      <c r="I275">
+      <c r="I275" s="2">
         <v>32.51</v>
       </c>
       <c r="J275">
@@ -16565,7 +16568,7 @@
       <c r="H276">
         <v>0.36</v>
       </c>
-      <c r="I276">
+      <c r="I276" s="2">
         <v>36.369999999999997</v>
       </c>
       <c r="J276">
@@ -16606,7 +16609,7 @@
       <c r="H277">
         <v>0.39</v>
       </c>
-      <c r="I277">
+      <c r="I277" s="2">
         <v>38.56</v>
       </c>
       <c r="J277">
@@ -16647,7 +16650,7 @@
       <c r="H278">
         <v>0.36</v>
       </c>
-      <c r="I278">
+      <c r="I278" s="2">
         <v>36</v>
       </c>
       <c r="J278">
@@ -16688,7 +16691,7 @@
       <c r="H279">
         <v>0.39</v>
       </c>
-      <c r="I279">
+      <c r="I279" s="2">
         <v>38.82</v>
       </c>
       <c r="J279">
@@ -16729,7 +16732,7 @@
       <c r="H280">
         <v>0.35</v>
       </c>
-      <c r="I280">
+      <c r="I280" s="2">
         <v>35.17</v>
       </c>
       <c r="J280">
@@ -16770,7 +16773,7 @@
       <c r="H281">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I281">
+      <c r="I281" s="2">
         <v>27.95</v>
       </c>
       <c r="J281">
@@ -16811,7 +16814,7 @@
       <c r="H282">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I282">
+      <c r="I282" s="2">
         <v>27.61</v>
       </c>
       <c r="J282">
@@ -16852,7 +16855,7 @@
       <c r="H283">
         <v>0.44</v>
       </c>
-      <c r="I283">
+      <c r="I283" s="2">
         <v>43.67</v>
       </c>
       <c r="J283">
@@ -16893,7 +16896,7 @@
       <c r="H284">
         <v>0.35</v>
       </c>
-      <c r="I284">
+      <c r="I284" s="2">
         <v>34.770000000000003</v>
       </c>
       <c r="J284">
@@ -16934,7 +16937,7 @@
       <c r="H285">
         <v>0.36</v>
       </c>
-      <c r="I285">
+      <c r="I285" s="2">
         <v>35.5</v>
       </c>
       <c r="J285">
@@ -16975,7 +16978,7 @@
       <c r="H286">
         <v>0.5</v>
       </c>
-      <c r="I286">
+      <c r="I286" s="2">
         <v>49.58</v>
       </c>
       <c r="J286">
@@ -17016,7 +17019,7 @@
       <c r="H287">
         <v>0.39</v>
       </c>
-      <c r="I287">
+      <c r="I287" s="2">
         <v>38.71</v>
       </c>
       <c r="J287">
@@ -17057,7 +17060,7 @@
       <c r="H288">
         <v>0.24</v>
       </c>
-      <c r="I288">
+      <c r="I288" s="2">
         <v>24.1</v>
       </c>
       <c r="J288">
@@ -17098,7 +17101,7 @@
       <c r="H289">
         <v>0.24</v>
       </c>
-      <c r="I289">
+      <c r="I289" s="2">
         <v>23.5</v>
       </c>
       <c r="J289">
@@ -17139,7 +17142,7 @@
       <c r="H290">
         <v>0.31</v>
       </c>
-      <c r="I290">
+      <c r="I290" s="2">
         <v>31.28</v>
       </c>
       <c r="J290">
@@ -17180,7 +17183,7 @@
       <c r="H291">
         <v>0.39</v>
       </c>
-      <c r="I291">
+      <c r="I291" s="2">
         <v>38.729999999999997</v>
       </c>
       <c r="J291">
@@ -17221,7 +17224,7 @@
       <c r="H292">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I292">
+      <c r="I292" s="2">
         <v>28.57</v>
       </c>
       <c r="J292">
@@ -17262,7 +17265,7 @@
       <c r="H293">
         <v>0.36</v>
       </c>
-      <c r="I293">
+      <c r="I293" s="2">
         <v>35.630000000000003</v>
       </c>
       <c r="J293">
@@ -17303,7 +17306,7 @@
       <c r="H294">
         <v>0.2</v>
       </c>
-      <c r="I294">
+      <c r="I294" s="2">
         <v>20</v>
       </c>
       <c r="J294">
@@ -17344,7 +17347,7 @@
       <c r="H295">
         <v>0.24</v>
       </c>
-      <c r="I295">
+      <c r="I295" s="2">
         <v>23.51</v>
       </c>
       <c r="J295">
@@ -17385,7 +17388,7 @@
       <c r="H296">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I296">
+      <c r="I296" s="2">
         <v>13.56</v>
       </c>
       <c r="J296">
@@ -17426,7 +17429,7 @@
       <c r="H297">
         <v>0.39</v>
       </c>
-      <c r="I297">
+      <c r="I297" s="2">
         <v>39.31</v>
       </c>
       <c r="J297">
@@ -17467,7 +17470,7 @@
       <c r="H298">
         <v>0.36</v>
       </c>
-      <c r="I298">
+      <c r="I298" s="2">
         <v>35.78</v>
       </c>
       <c r="J298">
@@ -17508,7 +17511,7 @@
       <c r="H299">
         <v>0</v>
       </c>
-      <c r="I299">
+      <c r="I299" s="2">
         <v>0</v>
       </c>
       <c r="J299">
@@ -17543,7 +17546,7 @@
       <c r="H300">
         <v>0</v>
       </c>
-      <c r="I300">
+      <c r="I300" s="2">
         <v>0</v>
       </c>
       <c r="J300">
@@ -17578,7 +17581,7 @@
       <c r="H301">
         <v>0.37</v>
       </c>
-      <c r="I301">
+      <c r="I301" s="2">
         <v>37.26</v>
       </c>
       <c r="J301">
@@ -17619,7 +17622,7 @@
       <c r="H302">
         <v>0.19</v>
       </c>
-      <c r="I302">
+      <c r="I302" s="2">
         <v>18.61</v>
       </c>
       <c r="J302">
@@ -17660,7 +17663,7 @@
       <c r="H303">
         <v>0.24</v>
       </c>
-      <c r="I303">
+      <c r="I303" s="2">
         <v>23.95</v>
       </c>
       <c r="J303">
@@ -17701,7 +17704,7 @@
       <c r="H304">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I304">
+      <c r="I304" s="2">
         <v>27.98</v>
       </c>
       <c r="J304">
@@ -17742,7 +17745,7 @@
       <c r="H305">
         <v>0</v>
       </c>
-      <c r="I305">
+      <c r="I305" s="2">
         <v>0</v>
       </c>
       <c r="J305">
@@ -17777,7 +17780,7 @@
       <c r="H306">
         <v>0.31</v>
       </c>
-      <c r="I306">
+      <c r="I306" s="2">
         <v>31.12</v>
       </c>
       <c r="J306">
@@ -17818,7 +17821,7 @@
       <c r="H307">
         <v>0.32</v>
       </c>
-      <c r="I307">
+      <c r="I307" s="2">
         <v>31.56</v>
       </c>
       <c r="J307">
@@ -17859,7 +17862,7 @@
       <c r="H308">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="I308">
+      <c r="I308" s="2">
         <v>7.25</v>
       </c>
       <c r="J308">
@@ -17900,7 +17903,7 @@
       <c r="H309">
         <v>0.36</v>
       </c>
-      <c r="I309">
+      <c r="I309" s="2">
         <v>36.29</v>
       </c>
       <c r="J309">
@@ -17941,7 +17944,7 @@
       <c r="H310">
         <v>0.27</v>
       </c>
-      <c r="I310">
+      <c r="I310" s="2">
         <v>26.66</v>
       </c>
       <c r="J310">
@@ -17982,7 +17985,7 @@
       <c r="H311">
         <v>0.13</v>
       </c>
-      <c r="I311">
+      <c r="I311" s="2">
         <v>13.46</v>
       </c>
       <c r="J311">
@@ -18023,7 +18026,7 @@
       <c r="H312">
         <v>0.26</v>
       </c>
-      <c r="I312">
+      <c r="I312" s="2">
         <v>25.51</v>
       </c>
       <c r="J312">
@@ -18064,7 +18067,7 @@
       <c r="H313">
         <v>0.31</v>
       </c>
-      <c r="I313">
+      <c r="I313" s="2">
         <v>30.93</v>
       </c>
       <c r="J313">
@@ -18105,7 +18108,7 @@
       <c r="H314">
         <v>0.37</v>
       </c>
-      <c r="I314">
+      <c r="I314" s="2">
         <v>37.26</v>
       </c>
       <c r="J314">
@@ -18146,7 +18149,7 @@
       <c r="H315">
         <v>0.25</v>
       </c>
-      <c r="I315">
+      <c r="I315" s="2">
         <v>25.24</v>
       </c>
       <c r="J315">
@@ -18187,7 +18190,7 @@
       <c r="H316">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I316">
+      <c r="I316" s="2">
         <v>29.13</v>
       </c>
       <c r="J316">
@@ -18228,7 +18231,7 @@
       <c r="H317">
         <v>0</v>
       </c>
-      <c r="I317">
+      <c r="I317" s="2">
         <v>0</v>
       </c>
       <c r="J317">
@@ -18263,7 +18266,7 @@
       <c r="H318">
         <v>0.61</v>
       </c>
-      <c r="I318">
+      <c r="I318" s="2">
         <v>61.4</v>
       </c>
       <c r="J318">
@@ -18304,7 +18307,7 @@
       <c r="H319">
         <v>0.38</v>
       </c>
-      <c r="I319">
+      <c r="I319" s="2">
         <v>38.46</v>
       </c>
       <c r="J319">
@@ -18345,7 +18348,7 @@
       <c r="H320">
         <v>0.33</v>
       </c>
-      <c r="I320">
+      <c r="I320" s="2">
         <v>33.47</v>
       </c>
       <c r="J320">
@@ -18386,7 +18389,7 @@
       <c r="H321">
         <v>0.48</v>
       </c>
-      <c r="I321">
+      <c r="I321" s="2">
         <v>48.11</v>
       </c>
       <c r="J321">
@@ -18427,7 +18430,7 @@
       <c r="H322">
         <v>0.34</v>
       </c>
-      <c r="I322">
+      <c r="I322" s="2">
         <v>34.119999999999997</v>
       </c>
       <c r="J322">
@@ -18468,7 +18471,7 @@
       <c r="H323">
         <v>0.46</v>
       </c>
-      <c r="I323">
+      <c r="I323" s="2">
         <v>45.76</v>
       </c>
       <c r="J323">
@@ -18509,7 +18512,7 @@
       <c r="H324">
         <v>0.32</v>
       </c>
-      <c r="I324">
+      <c r="I324" s="2">
         <v>32.35</v>
       </c>
       <c r="J324">
@@ -18550,7 +18553,7 @@
       <c r="H325">
         <v>0.48</v>
       </c>
-      <c r="I325">
+      <c r="I325" s="2">
         <v>48.15</v>
       </c>
       <c r="J325">
@@ -18591,7 +18594,7 @@
       <c r="H326">
         <v>0</v>
       </c>
-      <c r="I326">
+      <c r="I326" s="2">
         <v>0</v>
       </c>
       <c r="J326">
@@ -18626,7 +18629,7 @@
       <c r="H327">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I327">
+      <c r="I327" s="2">
         <v>28.23</v>
       </c>
       <c r="J327">
@@ -18667,7 +18670,7 @@
       <c r="H328">
         <v>0.36</v>
       </c>
-      <c r="I328">
+      <c r="I328" s="2">
         <v>35.65</v>
       </c>
       <c r="J328">
@@ -18708,7 +18711,7 @@
       <c r="H329">
         <v>0.35</v>
       </c>
-      <c r="I329">
+      <c r="I329" s="2">
         <v>34.97</v>
       </c>
       <c r="J329">
@@ -18749,7 +18752,7 @@
       <c r="H330">
         <v>0.46</v>
       </c>
-      <c r="I330">
+      <c r="I330" s="2">
         <v>45.83</v>
       </c>
       <c r="J330">
@@ -18790,7 +18793,7 @@
       <c r="H331">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I331">
+      <c r="I331" s="2">
         <v>29.39</v>
       </c>
       <c r="J331">
@@ -18831,7 +18834,7 @@
       <c r="H332">
         <v>0.39</v>
       </c>
-      <c r="I332">
+      <c r="I332" s="2">
         <v>39.119999999999997</v>
       </c>
       <c r="J332">
@@ -18872,7 +18875,7 @@
       <c r="H333">
         <v>0.34</v>
       </c>
-      <c r="I333">
+      <c r="I333" s="2">
         <v>34.26</v>
       </c>
       <c r="J333">
@@ -18913,7 +18916,7 @@
       <c r="H334">
         <v>0.25</v>
       </c>
-      <c r="I334">
+      <c r="I334" s="2">
         <v>25.07</v>
       </c>
       <c r="J334">
@@ -18954,7 +18957,7 @@
       <c r="H335">
         <v>0.31</v>
       </c>
-      <c r="I335">
+      <c r="I335" s="2">
         <v>30.66</v>
       </c>
       <c r="J335">
@@ -18995,7 +18998,7 @@
       <c r="H336">
         <v>0.34</v>
       </c>
-      <c r="I336">
+      <c r="I336" s="2">
         <v>33.85</v>
       </c>
       <c r="J336">
@@ -19036,7 +19039,7 @@
       <c r="H337">
         <v>0</v>
       </c>
-      <c r="I337">
+      <c r="I337" s="2">
         <v>0</v>
       </c>
       <c r="J337">
@@ -19071,7 +19074,7 @@
       <c r="H338">
         <v>0.21</v>
       </c>
-      <c r="I338">
+      <c r="I338" s="2">
         <v>21.46</v>
       </c>
       <c r="J338">
@@ -19112,7 +19115,7 @@
       <c r="H339">
         <v>0.45</v>
       </c>
-      <c r="I339">
+      <c r="I339" s="2">
         <v>44.99</v>
       </c>
       <c r="J339">
@@ -19153,7 +19156,7 @@
       <c r="H340">
         <v>0</v>
       </c>
-      <c r="I340">
+      <c r="I340" s="2">
         <v>0</v>
       </c>
       <c r="J340">
@@ -19188,7 +19191,7 @@
       <c r="H341">
         <v>0.37</v>
       </c>
-      <c r="I341">
+      <c r="I341" s="2">
         <v>36.99</v>
       </c>
       <c r="J341">
@@ -19229,7 +19232,7 @@
       <c r="H342">
         <v>0.27</v>
       </c>
-      <c r="I342">
+      <c r="I342" s="2">
         <v>27.15</v>
       </c>
       <c r="J342">
@@ -19270,7 +19273,7 @@
       <c r="H343">
         <v>0.34</v>
       </c>
-      <c r="I343">
+      <c r="I343" s="2">
         <v>33.979999999999997</v>
       </c>
       <c r="J343">
@@ -19311,7 +19314,7 @@
       <c r="H344">
         <v>0.61</v>
       </c>
-      <c r="I344">
+      <c r="I344" s="2">
         <v>61.4</v>
       </c>
       <c r="J344">
@@ -19352,7 +19355,7 @@
       <c r="H345">
         <v>0.34</v>
       </c>
-      <c r="I345">
+      <c r="I345" s="2">
         <v>33.880000000000003</v>
       </c>
       <c r="J345">
@@ -19393,7 +19396,7 @@
       <c r="H346">
         <v>0.25</v>
       </c>
-      <c r="I346">
+      <c r="I346" s="2">
         <v>25.08</v>
       </c>
       <c r="J346">
@@ -19434,7 +19437,7 @@
       <c r="H347">
         <v>0.35</v>
       </c>
-      <c r="I347">
+      <c r="I347" s="2">
         <v>34.979999999999997</v>
       </c>
       <c r="J347">
@@ -19475,7 +19478,7 @@
       <c r="H348">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I348">
+      <c r="I348" s="2">
         <v>28.45</v>
       </c>
       <c r="J348">
@@ -19516,7 +19519,7 @@
       <c r="H349">
         <v>0.49</v>
       </c>
-      <c r="I349">
+      <c r="I349" s="2">
         <v>48.97</v>
       </c>
       <c r="J349">
@@ -19557,7 +19560,7 @@
       <c r="H350">
         <v>0.39</v>
       </c>
-      <c r="I350">
+      <c r="I350" s="2">
         <v>39.07</v>
       </c>
       <c r="J350">
@@ -19598,7 +19601,7 @@
       <c r="H351">
         <v>0.18</v>
       </c>
-      <c r="I351">
+      <c r="I351" s="2">
         <v>17.79</v>
       </c>
       <c r="J351">
@@ -19639,7 +19642,7 @@
       <c r="H352">
         <v>0.37</v>
       </c>
-      <c r="I352">
+      <c r="I352" s="2">
         <v>36.54</v>
       </c>
       <c r="J352">
@@ -19680,7 +19683,7 @@
       <c r="H353">
         <v>0.53</v>
       </c>
-      <c r="I353">
+      <c r="I353" s="2">
         <v>52.87</v>
       </c>
       <c r="J353">
@@ -19721,7 +19724,7 @@
       <c r="H354">
         <v>0.35</v>
       </c>
-      <c r="I354">
+      <c r="I354" s="2">
         <v>34.71</v>
       </c>
       <c r="J354">
@@ -19762,7 +19765,7 @@
       <c r="H355">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I355">
+      <c r="I355" s="2">
         <v>28.32</v>
       </c>
       <c r="J355">
@@ -19803,7 +19806,7 @@
       <c r="H356">
         <v>0.18</v>
       </c>
-      <c r="I356">
+      <c r="I356" s="2">
         <v>17.829999999999998</v>
       </c>
       <c r="J356">
@@ -19844,7 +19847,7 @@
       <c r="H357">
         <v>0.31</v>
       </c>
-      <c r="I357">
+      <c r="I357" s="2">
         <v>31.25</v>
       </c>
       <c r="J357">
@@ -19885,7 +19888,7 @@
       <c r="H358">
         <v>0.23</v>
       </c>
-      <c r="I358">
+      <c r="I358" s="2">
         <v>23.39</v>
       </c>
       <c r="J358">
@@ -19926,7 +19929,7 @@
       <c r="H359">
         <v>0.21</v>
       </c>
-      <c r="I359">
+      <c r="I359" s="2">
         <v>21.11</v>
       </c>
       <c r="J359">
@@ -19967,7 +19970,7 @@
       <c r="H360">
         <v>0.34</v>
       </c>
-      <c r="I360">
+      <c r="I360" s="2">
         <v>34.47</v>
       </c>
       <c r="J360">
@@ -20008,7 +20011,7 @@
       <c r="H361">
         <v>0.23</v>
       </c>
-      <c r="I361">
+      <c r="I361" s="2">
         <v>23.05</v>
       </c>
       <c r="J361">
@@ -20049,7 +20052,7 @@
       <c r="H362">
         <v>0.36</v>
       </c>
-      <c r="I362">
+      <c r="I362" s="2">
         <v>36.299999999999997</v>
       </c>
       <c r="J362">
@@ -20090,7 +20093,7 @@
       <c r="H363">
         <v>0.17</v>
       </c>
-      <c r="I363">
+      <c r="I363" s="2">
         <v>16.510000000000002</v>
       </c>
       <c r="J363">
@@ -20131,7 +20134,7 @@
       <c r="H364">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I364">
+      <c r="I364" s="2">
         <v>27.88</v>
       </c>
       <c r="J364">
@@ -20172,7 +20175,7 @@
       <c r="H365">
         <v>0.22</v>
       </c>
-      <c r="I365">
+      <c r="I365" s="2">
         <v>21.54</v>
       </c>
       <c r="J365">
@@ -20213,7 +20216,7 @@
       <c r="H366">
         <v>0.41</v>
       </c>
-      <c r="I366">
+      <c r="I366" s="2">
         <v>41.24</v>
       </c>
       <c r="J366">
@@ -20254,7 +20257,7 @@
       <c r="H367">
         <v>0.24</v>
       </c>
-      <c r="I367">
+      <c r="I367" s="2">
         <v>24.33</v>
       </c>
       <c r="J367">
@@ -20295,7 +20298,7 @@
       <c r="H368">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I368">
+      <c r="I368" s="2">
         <v>14.2</v>
       </c>
       <c r="J368">
@@ -20336,7 +20339,7 @@
       <c r="H369">
         <v>0.26</v>
       </c>
-      <c r="I369">
+      <c r="I369" s="2">
         <v>25.59</v>
       </c>
       <c r="J369">
@@ -20377,7 +20380,7 @@
       <c r="H370">
         <v>0.22</v>
       </c>
-      <c r="I370">
+      <c r="I370" s="2">
         <v>22.18</v>
       </c>
       <c r="J370">
@@ -20418,7 +20421,7 @@
       <c r="H371">
         <v>0.45</v>
       </c>
-      <c r="I371">
+      <c r="I371" s="2">
         <v>45.48</v>
       </c>
       <c r="J371">
@@ -20459,7 +20462,7 @@
       <c r="H372">
         <v>0.17</v>
       </c>
-      <c r="I372">
+      <c r="I372" s="2">
         <v>16.93</v>
       </c>
       <c r="J372">
@@ -20500,7 +20503,7 @@
       <c r="H373">
         <v>0.11</v>
       </c>
-      <c r="I373">
+      <c r="I373" s="2">
         <v>10.96</v>
       </c>
       <c r="J373">
@@ -20541,7 +20544,7 @@
       <c r="H374">
         <v>0.23</v>
       </c>
-      <c r="I374">
+      <c r="I374" s="2">
         <v>23.27</v>
       </c>
       <c r="J374">
@@ -20582,7 +20585,7 @@
       <c r="H375">
         <v>0</v>
       </c>
-      <c r="I375">
+      <c r="I375" s="2">
         <v>0</v>
       </c>
       <c r="J375">
@@ -20617,7 +20620,7 @@
       <c r="H376">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I376">
+      <c r="I376" s="2">
         <v>29.47</v>
       </c>
       <c r="J376">
@@ -20658,7 +20661,7 @@
       <c r="H377">
         <v>0.31</v>
       </c>
-      <c r="I377">
+      <c r="I377" s="2">
         <v>30.54</v>
       </c>
       <c r="J377">
@@ -20699,7 +20702,7 @@
       <c r="H378">
         <v>0.34</v>
       </c>
-      <c r="I378">
+      <c r="I378" s="2">
         <v>33.619999999999997</v>
       </c>
       <c r="J378">
@@ -20740,7 +20743,7 @@
       <c r="H379">
         <v>0.32</v>
       </c>
-      <c r="I379">
+      <c r="I379" s="2">
         <v>32.03</v>
       </c>
       <c r="J379">
@@ -20781,7 +20784,7 @@
       <c r="H380">
         <v>0.4</v>
       </c>
-      <c r="I380">
+      <c r="I380" s="2">
         <v>39.99</v>
       </c>
       <c r="J380">
@@ -20822,7 +20825,7 @@
       <c r="H381">
         <v>0.26</v>
       </c>
-      <c r="I381">
+      <c r="I381" s="2">
         <v>26.32</v>
       </c>
       <c r="J381">
@@ -20863,7 +20866,7 @@
       <c r="H382">
         <v>0.25</v>
       </c>
-      <c r="I382">
+      <c r="I382" s="2">
         <v>25.27</v>
       </c>
       <c r="J382">
@@ -20904,7 +20907,7 @@
       <c r="H383">
         <v>0.21</v>
       </c>
-      <c r="I383">
+      <c r="I383" s="2">
         <v>21</v>
       </c>
       <c r="J383">
@@ -20945,7 +20948,7 @@
       <c r="H384">
         <v>0.39</v>
       </c>
-      <c r="I384">
+      <c r="I384" s="2">
         <v>38.799999999999997</v>
       </c>
       <c r="J384">
@@ -20986,7 +20989,7 @@
       <c r="H385">
         <v>0.33</v>
       </c>
-      <c r="I385">
+      <c r="I385" s="2">
         <v>32.630000000000003</v>
       </c>
       <c r="J385">
@@ -21027,7 +21030,7 @@
       <c r="H386">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I386">
+      <c r="I386" s="2">
         <v>27.9</v>
       </c>
       <c r="J386">
@@ -21068,7 +21071,7 @@
       <c r="H387">
         <v>0.3</v>
       </c>
-      <c r="I387">
+      <c r="I387" s="2">
         <v>29.82</v>
       </c>
       <c r="J387">
@@ -21109,7 +21112,7 @@
       <c r="H388">
         <v>0.32</v>
       </c>
-      <c r="I388">
+      <c r="I388" s="2">
         <v>31.64</v>
       </c>
       <c r="J388">
@@ -21150,7 +21153,7 @@
       <c r="H389">
         <v>0.3</v>
       </c>
-      <c r="I389">
+      <c r="I389" s="2">
         <v>29.91</v>
       </c>
       <c r="J389">
@@ -21191,7 +21194,7 @@
       <c r="H390">
         <v>0.35</v>
       </c>
-      <c r="I390">
+      <c r="I390" s="2">
         <v>35.020000000000003</v>
       </c>
       <c r="J390">
@@ -21232,7 +21235,7 @@
       <c r="H391">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I391">
+      <c r="I391" s="2">
         <v>28.69</v>
       </c>
       <c r="J391">
@@ -21273,7 +21276,7 @@
       <c r="H392">
         <v>0</v>
       </c>
-      <c r="I392">
+      <c r="I392" s="2">
         <v>0</v>
       </c>
       <c r="J392">
@@ -21308,7 +21311,7 @@
       <c r="H393">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I393">
+      <c r="I393" s="2">
         <v>28.87</v>
       </c>
       <c r="J393">
@@ -21349,7 +21352,7 @@
       <c r="H394">
         <v>0.26</v>
       </c>
-      <c r="I394">
+      <c r="I394" s="2">
         <v>25.73</v>
       </c>
       <c r="J394">
@@ -21390,7 +21393,7 @@
       <c r="H395">
         <v>0.15</v>
       </c>
-      <c r="I395">
+      <c r="I395" s="2">
         <v>15.15</v>
       </c>
       <c r="J395">
@@ -21431,7 +21434,7 @@
       <c r="H396">
         <v>0.33</v>
       </c>
-      <c r="I396">
+      <c r="I396" s="2">
         <v>32.590000000000003</v>
       </c>
       <c r="J396">
@@ -21472,7 +21475,7 @@
       <c r="H397">
         <v>0.27</v>
       </c>
-      <c r="I397">
+      <c r="I397" s="2">
         <v>27.37</v>
       </c>
       <c r="J397">
@@ -21513,7 +21516,7 @@
       <c r="H398">
         <v>0.22</v>
       </c>
-      <c r="I398">
+      <c r="I398" s="2">
         <v>21.77</v>
       </c>
       <c r="J398">
@@ -21554,7 +21557,7 @@
       <c r="H399">
         <v>0.42</v>
       </c>
-      <c r="I399">
+      <c r="I399" s="2">
         <v>41.93</v>
       </c>
       <c r="J399">
@@ -21595,7 +21598,7 @@
       <c r="H400">
         <v>0.32</v>
       </c>
-      <c r="I400">
+      <c r="I400" s="2">
         <v>32.380000000000003</v>
       </c>
       <c r="J400">
@@ -21636,7 +21639,7 @@
       <c r="H401">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I401">
+      <c r="I401" s="2">
         <v>28.56</v>
       </c>
       <c r="J401">
@@ -21677,7 +21680,7 @@
       <c r="H402">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I402">
+      <c r="I402" s="2">
         <v>28.28</v>
       </c>
       <c r="J402">
@@ -21718,7 +21721,7 @@
       <c r="H403">
         <v>0.3</v>
       </c>
-      <c r="I403">
+      <c r="I403" s="2">
         <v>29.58</v>
       </c>
       <c r="J403">
@@ -21759,7 +21762,7 @@
       <c r="H404">
         <v>0.24</v>
       </c>
-      <c r="I404">
+      <c r="I404" s="2">
         <v>24.28</v>
       </c>
       <c r="J404">
@@ -21800,7 +21803,7 @@
       <c r="H405">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I405">
+      <c r="I405" s="2">
         <v>28.48</v>
       </c>
       <c r="J405">
@@ -21841,7 +21844,7 @@
       <c r="H406">
         <v>0</v>
       </c>
-      <c r="I406">
+      <c r="I406" s="2">
         <v>0</v>
       </c>
       <c r="J406">
@@ -21876,7 +21879,7 @@
       <c r="H407">
         <v>0.34</v>
       </c>
-      <c r="I407">
+      <c r="I407" s="2">
         <v>34.21</v>
       </c>
       <c r="J407">
@@ -21917,7 +21920,7 @@
       <c r="H408">
         <v>0.44</v>
       </c>
-      <c r="I408">
+      <c r="I408" s="2">
         <v>43.91</v>
       </c>
       <c r="J408">
@@ -21958,7 +21961,7 @@
       <c r="H409">
         <v>0.33</v>
       </c>
-      <c r="I409">
+      <c r="I409" s="2">
         <v>33.47</v>
       </c>
       <c r="J409">
@@ -21999,7 +22002,7 @@
       <c r="H410">
         <v>0.37</v>
       </c>
-      <c r="I410">
+      <c r="I410" s="2">
         <v>37.49</v>
       </c>
       <c r="J410">
@@ -22040,7 +22043,7 @@
       <c r="H411">
         <v>0.32</v>
       </c>
-      <c r="I411">
+      <c r="I411" s="2">
         <v>31.81</v>
       </c>
       <c r="J411">
@@ -22081,7 +22084,7 @@
       <c r="H412">
         <v>0.52</v>
       </c>
-      <c r="I412">
+      <c r="I412" s="2">
         <v>51.77</v>
       </c>
       <c r="J412">
@@ -22122,7 +22125,7 @@
       <c r="H413">
         <v>0.25</v>
       </c>
-      <c r="I413">
+      <c r="I413" s="2">
         <v>25.09</v>
       </c>
       <c r="J413">
@@ -22163,7 +22166,7 @@
       <c r="H414">
         <v>0.36</v>
       </c>
-      <c r="I414">
+      <c r="I414" s="2">
         <v>36.29</v>
       </c>
       <c r="J414">
@@ -22204,7 +22207,7 @@
       <c r="H415">
         <v>0.32</v>
       </c>
-      <c r="I415">
+      <c r="I415" s="2">
         <v>32.380000000000003</v>
       </c>
       <c r="J415">
@@ -22245,7 +22248,7 @@
       <c r="H416">
         <v>0.38</v>
       </c>
-      <c r="I416">
+      <c r="I416" s="2">
         <v>37.51</v>
       </c>
       <c r="J416">
@@ -22286,7 +22289,7 @@
       <c r="H417">
         <v>0.33</v>
       </c>
-      <c r="I417">
+      <c r="I417" s="2">
         <v>33.22</v>
       </c>
       <c r="J417">
@@ -22327,7 +22330,7 @@
       <c r="H418">
         <v>0.31</v>
       </c>
-      <c r="I418">
+      <c r="I418" s="2">
         <v>31.11</v>
       </c>
       <c r="J418">
@@ -22368,7 +22371,7 @@
       <c r="H419">
         <v>0.25</v>
       </c>
-      <c r="I419">
+      <c r="I419" s="2">
         <v>24.94</v>
       </c>
       <c r="J419">
@@ -22409,7 +22412,7 @@
       <c r="H420">
         <v>0.36</v>
       </c>
-      <c r="I420">
+      <c r="I420" s="2">
         <v>35.909999999999997</v>
       </c>
       <c r="J420">
@@ -22450,7 +22453,7 @@
       <c r="H421">
         <v>0.34</v>
       </c>
-      <c r="I421">
+      <c r="I421" s="2">
         <v>34.14</v>
       </c>
       <c r="J421">
@@ -22491,7 +22494,7 @@
       <c r="H422">
         <v>0.4</v>
       </c>
-      <c r="I422">
+      <c r="I422" s="2">
         <v>40.130000000000003</v>
       </c>
       <c r="J422">
@@ -22532,7 +22535,7 @@
       <c r="H423">
         <v>0</v>
       </c>
-      <c r="I423">
+      <c r="I423" s="2">
         <v>0</v>
       </c>
       <c r="J423">
@@ -22567,7 +22570,7 @@
       <c r="H424">
         <v>0.41</v>
       </c>
-      <c r="I424">
+      <c r="I424" s="2">
         <v>40.61</v>
       </c>
       <c r="J424">
@@ -22608,7 +22611,7 @@
       <c r="H425">
         <v>0.34</v>
       </c>
-      <c r="I425">
+      <c r="I425" s="2">
         <v>33.950000000000003</v>
       </c>
       <c r="J425">
@@ -22649,7 +22652,7 @@
       <c r="H426">
         <v>0.32</v>
       </c>
-      <c r="I426">
+      <c r="I426" s="2">
         <v>32.4</v>
       </c>
       <c r="J426">
@@ -22690,7 +22693,7 @@
       <c r="H427">
         <v>0.61</v>
       </c>
-      <c r="I427">
+      <c r="I427" s="2">
         <v>61.4</v>
       </c>
       <c r="J427">
@@ -22731,7 +22734,7 @@
       <c r="H428">
         <v>0.34</v>
       </c>
-      <c r="I428">
+      <c r="I428" s="2">
         <v>34.369999999999997</v>
       </c>
       <c r="J428">
@@ -22772,7 +22775,7 @@
       <c r="H429">
         <v>0.42</v>
       </c>
-      <c r="I429">
+      <c r="I429" s="2">
         <v>41.67</v>
       </c>
       <c r="J429">
@@ -22813,7 +22816,7 @@
       <c r="H430">
         <v>0.35</v>
       </c>
-      <c r="I430">
+      <c r="I430" s="2">
         <v>35.020000000000003</v>
       </c>
       <c r="J430">
@@ -22854,7 +22857,7 @@
       <c r="H431">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I431">
+      <c r="I431" s="2">
         <v>29.46</v>
       </c>
       <c r="J431">
@@ -22895,7 +22898,7 @@
       <c r="H432">
         <v>0</v>
       </c>
-      <c r="I432">
+      <c r="I432" s="2">
         <v>0</v>
       </c>
       <c r="J432">
@@ -22930,7 +22933,7 @@
       <c r="H433">
         <v>0.24</v>
       </c>
-      <c r="I433">
+      <c r="I433" s="2">
         <v>23.72</v>
       </c>
       <c r="J433">
@@ -22971,7 +22974,7 @@
       <c r="H434">
         <v>0.27</v>
       </c>
-      <c r="I434">
+      <c r="I434" s="2">
         <v>27.04</v>
       </c>
       <c r="J434">
@@ -23012,7 +23015,7 @@
       <c r="H435">
         <v>0.39</v>
       </c>
-      <c r="I435">
+      <c r="I435" s="2">
         <v>39.119999999999997</v>
       </c>
       <c r="J435">
@@ -23053,7 +23056,7 @@
       <c r="H436">
         <v>0.24</v>
       </c>
-      <c r="I436">
+      <c r="I436" s="2">
         <v>23.62</v>
       </c>
       <c r="J436">
@@ -23094,7 +23097,7 @@
       <c r="H437">
         <v>0.31</v>
       </c>
-      <c r="I437">
+      <c r="I437" s="2">
         <v>30.87</v>
       </c>
       <c r="J437">
@@ -23135,7 +23138,7 @@
       <c r="H438">
         <v>0</v>
       </c>
-      <c r="I438">
+      <c r="I438" s="2">
         <v>0</v>
       </c>
       <c r="J438">
@@ -23170,7 +23173,7 @@
       <c r="H439">
         <v>0.38</v>
       </c>
-      <c r="I439">
+      <c r="I439" s="2">
         <v>38.49</v>
       </c>
       <c r="J439">
@@ -23211,7 +23214,7 @@
       <c r="H440">
         <v>0.31</v>
       </c>
-      <c r="I440">
+      <c r="I440" s="2">
         <v>30.85</v>
       </c>
       <c r="J440">
@@ -23252,7 +23255,7 @@
       <c r="H441">
         <v>0.41</v>
       </c>
-      <c r="I441">
+      <c r="I441" s="2">
         <v>41.34</v>
       </c>
       <c r="J441">
@@ -23293,7 +23296,7 @@
       <c r="H442">
         <v>0.32</v>
       </c>
-      <c r="I442">
+      <c r="I442" s="2">
         <v>32.47</v>
       </c>
       <c r="J442">
@@ -23334,7 +23337,7 @@
       <c r="H443">
         <v>0.3</v>
       </c>
-      <c r="I443">
+      <c r="I443" s="2">
         <v>29.64</v>
       </c>
       <c r="J443">
@@ -23375,7 +23378,7 @@
       <c r="H444">
         <v>0.36</v>
       </c>
-      <c r="I444">
+      <c r="I444" s="2">
         <v>36.19</v>
       </c>
       <c r="J444">
@@ -23416,7 +23419,7 @@
       <c r="H445">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I445">
+      <c r="I445" s="2">
         <v>29.09</v>
       </c>
       <c r="J445">
@@ -23457,7 +23460,7 @@
       <c r="H446">
         <v>0.22</v>
       </c>
-      <c r="I446">
+      <c r="I446" s="2">
         <v>22.3</v>
       </c>
       <c r="J446">
@@ -23498,7 +23501,7 @@
       <c r="H447">
         <v>0.35</v>
       </c>
-      <c r="I447">
+      <c r="I447" s="2">
         <v>34.979999999999997</v>
       </c>
       <c r="J447">
@@ -23539,7 +23542,7 @@
       <c r="H448">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I448">
+      <c r="I448" s="2">
         <v>28.98</v>
       </c>
       <c r="J448">
@@ -23580,7 +23583,7 @@
       <c r="H449">
         <v>0.32</v>
       </c>
-      <c r="I449">
+      <c r="I449" s="2">
         <v>32.07</v>
       </c>
       <c r="J449">
@@ -23621,7 +23624,7 @@
       <c r="H450">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I450">
+      <c r="I450" s="2">
         <v>28.47</v>
       </c>
       <c r="J450">
@@ -23662,7 +23665,7 @@
       <c r="H451">
         <v>0.15</v>
       </c>
-      <c r="I451">
+      <c r="I451" s="2">
         <v>14.68</v>
       </c>
       <c r="J451">
@@ -23703,7 +23706,7 @@
       <c r="H452">
         <v>0.41</v>
       </c>
-      <c r="I452">
+      <c r="I452" s="2">
         <v>41.16</v>
       </c>
       <c r="J452">
@@ -23744,7 +23747,7 @@
       <c r="H453">
         <v>0.35</v>
       </c>
-      <c r="I453">
+      <c r="I453" s="2">
         <v>34.96</v>
       </c>
       <c r="J453">
@@ -23785,7 +23788,7 @@
       <c r="H454">
         <v>0.25</v>
       </c>
-      <c r="I454">
+      <c r="I454" s="2">
         <v>25.19</v>
       </c>
       <c r="J454">
@@ -23826,7 +23829,7 @@
       <c r="H455">
         <v>0.25</v>
       </c>
-      <c r="I455">
+      <c r="I455" s="2">
         <v>24.56</v>
       </c>
       <c r="J455">
@@ -23867,7 +23870,7 @@
       <c r="H456">
         <v>0.24</v>
       </c>
-      <c r="I456">
+      <c r="I456" s="2">
         <v>24.2</v>
       </c>
       <c r="J456">
@@ -23908,7 +23911,7 @@
       <c r="H457">
         <v>0</v>
       </c>
-      <c r="I457">
+      <c r="I457" s="2">
         <v>0</v>
       </c>
       <c r="J457">
@@ -23943,7 +23946,7 @@
       <c r="H458">
         <v>0.42</v>
       </c>
-      <c r="I458">
+      <c r="I458" s="2">
         <v>41.88</v>
       </c>
       <c r="J458">
@@ -23984,7 +23987,7 @@
       <c r="H459">
         <v>0.39</v>
       </c>
-      <c r="I459">
+      <c r="I459" s="2">
         <v>39.32</v>
       </c>
       <c r="J459">
@@ -24025,7 +24028,7 @@
       <c r="H460">
         <v>0.32</v>
       </c>
-      <c r="I460">
+      <c r="I460" s="2">
         <v>31.59</v>
       </c>
       <c r="J460">
@@ -24066,7 +24069,7 @@
       <c r="H461">
         <v>0.45</v>
       </c>
-      <c r="I461">
+      <c r="I461" s="2">
         <v>44.86</v>
       </c>
       <c r="J461">
@@ -24107,7 +24110,7 @@
       <c r="H462">
         <v>0.39</v>
       </c>
-      <c r="I462">
+      <c r="I462" s="2">
         <v>39.04</v>
       </c>
       <c r="J462">
@@ -24148,7 +24151,7 @@
       <c r="H463">
         <v>0.37</v>
       </c>
-      <c r="I463">
+      <c r="I463" s="2">
         <v>36.5</v>
       </c>
       <c r="J463">
@@ -24189,7 +24192,7 @@
       <c r="H464">
         <v>0.39</v>
       </c>
-      <c r="I464">
+      <c r="I464" s="2">
         <v>39.28</v>
       </c>
       <c r="J464">
@@ -24230,7 +24233,7 @@
       <c r="H465">
         <v>0.36</v>
       </c>
-      <c r="I465">
+      <c r="I465" s="2">
         <v>35.74</v>
       </c>
       <c r="J465">
@@ -24271,7 +24274,7 @@
       <c r="H466">
         <v>0.36</v>
       </c>
-      <c r="I466">
+      <c r="I466" s="2">
         <v>35.590000000000003</v>
       </c>
       <c r="J466">
@@ -24312,7 +24315,7 @@
       <c r="H467">
         <v>0.42</v>
       </c>
-      <c r="I467">
+      <c r="I467" s="2">
         <v>41.75</v>
       </c>
       <c r="J467">
@@ -24353,7 +24356,7 @@
       <c r="H468">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I468">
+      <c r="I468" s="2">
         <v>28.69</v>
       </c>
       <c r="J468">
@@ -24394,7 +24397,7 @@
       <c r="H469">
         <v>0.35</v>
       </c>
-      <c r="I469">
+      <c r="I469" s="2">
         <v>34.89</v>
       </c>
       <c r="J469">
@@ -24435,7 +24438,7 @@
       <c r="H470">
         <v>0.37</v>
       </c>
-      <c r="I470">
+      <c r="I470" s="2">
         <v>37.42</v>
       </c>
       <c r="J470">
@@ -24476,7 +24479,7 @@
       <c r="H471">
         <v>0.35</v>
       </c>
-      <c r="I471">
+      <c r="I471" s="2">
         <v>35.5</v>
       </c>
       <c r="J471">
@@ -24517,7 +24520,7 @@
       <c r="H472">
         <v>0.34</v>
       </c>
-      <c r="I472">
+      <c r="I472" s="2">
         <v>34.4</v>
       </c>
       <c r="J472">
@@ -24558,7 +24561,7 @@
       <c r="H473">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I473">
+      <c r="I473" s="2">
         <v>27.55</v>
       </c>
       <c r="J473">
@@ -24599,7 +24602,7 @@
       <c r="H474">
         <v>0.36</v>
       </c>
-      <c r="I474">
+      <c r="I474" s="2">
         <v>36.299999999999997</v>
       </c>
       <c r="J474">
@@ -24640,7 +24643,7 @@
       <c r="H475">
         <v>0.37</v>
       </c>
-      <c r="I475">
+      <c r="I475" s="2">
         <v>37.479999999999997</v>
       </c>
       <c r="J475">
@@ -24681,7 +24684,7 @@
       <c r="H476">
         <v>0.31</v>
       </c>
-      <c r="I476">
+      <c r="I476" s="2">
         <v>31.02</v>
       </c>
       <c r="J476">
@@ -24722,7 +24725,7 @@
       <c r="H477">
         <v>0.43</v>
       </c>
-      <c r="I477">
+      <c r="I477" s="2">
         <v>42.69</v>
       </c>
       <c r="J477">
@@ -24763,7 +24766,7 @@
       <c r="H478">
         <v>0.43</v>
       </c>
-      <c r="I478">
+      <c r="I478" s="2">
         <v>42.79</v>
       </c>
       <c r="J478">
@@ -24804,7 +24807,7 @@
       <c r="H479">
         <v>0.35</v>
       </c>
-      <c r="I479">
+      <c r="I479" s="2">
         <v>34.93</v>
       </c>
       <c r="J479">
@@ -24845,7 +24848,7 @@
       <c r="H480">
         <v>0.32</v>
       </c>
-      <c r="I480">
+      <c r="I480" s="2">
         <v>32.450000000000003</v>
       </c>
       <c r="J480">
@@ -24886,7 +24889,7 @@
       <c r="H481">
         <v>0.42</v>
       </c>
-      <c r="I481">
+      <c r="I481" s="2">
         <v>42.43</v>
       </c>
       <c r="J481">
@@ -24927,7 +24930,7 @@
       <c r="H482">
         <v>0</v>
       </c>
-      <c r="I482">
+      <c r="I482" s="2">
         <v>0</v>
       </c>
       <c r="J482">
@@ -24962,7 +24965,7 @@
       <c r="H483">
         <v>0.36</v>
       </c>
-      <c r="I483">
+      <c r="I483" s="2">
         <v>35.71</v>
       </c>
       <c r="J483">
@@ -25003,7 +25006,7 @@
       <c r="H484">
         <v>0.36</v>
       </c>
-      <c r="I484">
+      <c r="I484" s="2">
         <v>35.92</v>
       </c>
       <c r="J484">
@@ -25044,7 +25047,7 @@
       <c r="H485">
         <v>0.33</v>
       </c>
-      <c r="I485">
+      <c r="I485" s="2">
         <v>32.78</v>
       </c>
       <c r="J485">
@@ -25085,7 +25088,7 @@
       <c r="H486">
         <v>0.39</v>
       </c>
-      <c r="I486">
+      <c r="I486" s="2">
         <v>38.96</v>
       </c>
       <c r="J486">
@@ -25126,7 +25129,7 @@
       <c r="H487">
         <v>0.53</v>
       </c>
-      <c r="I487">
+      <c r="I487" s="2">
         <v>53.03</v>
       </c>
       <c r="J487">
@@ -25167,7 +25170,7 @@
       <c r="H488">
         <v>0.43</v>
       </c>
-      <c r="I488">
+      <c r="I488" s="2">
         <v>43.21</v>
       </c>
       <c r="J488">
@@ -25208,7 +25211,7 @@
       <c r="H489">
         <v>0.33</v>
       </c>
-      <c r="I489">
+      <c r="I489" s="2">
         <v>33.28</v>
       </c>
       <c r="J489">
@@ -25249,7 +25252,7 @@
       <c r="H490">
         <v>0.26</v>
       </c>
-      <c r="I490">
+      <c r="I490" s="2">
         <v>26.1</v>
       </c>
       <c r="J490">
@@ -25290,7 +25293,7 @@
       <c r="H491">
         <v>0.35</v>
       </c>
-      <c r="I491">
+      <c r="I491" s="2">
         <v>35.01</v>
       </c>
       <c r="J491">
@@ -25331,7 +25334,7 @@
       <c r="H492">
         <v>0.43</v>
       </c>
-      <c r="I492">
+      <c r="I492" s="2">
         <v>43.45</v>
       </c>
       <c r="J492">
@@ -25372,7 +25375,7 @@
       <c r="H493">
         <v>0.38</v>
       </c>
-      <c r="I493">
+      <c r="I493" s="2">
         <v>38.47</v>
       </c>
       <c r="J493">
@@ -25413,7 +25416,7 @@
       <c r="H494">
         <v>0.24</v>
       </c>
-      <c r="I494">
+      <c r="I494" s="2">
         <v>24.48</v>
       </c>
       <c r="J494">
@@ -25454,7 +25457,7 @@
       <c r="H495">
         <v>0.46</v>
       </c>
-      <c r="I495">
+      <c r="I495" s="2">
         <v>45.66</v>
       </c>
       <c r="J495">
@@ -25495,7 +25498,7 @@
       <c r="H496">
         <v>0.61</v>
       </c>
-      <c r="I496">
+      <c r="I496" s="2">
         <v>61.4</v>
       </c>
       <c r="J496">
@@ -25536,7 +25539,7 @@
       <c r="H497">
         <v>0.48</v>
       </c>
-      <c r="I497">
+      <c r="I497" s="2">
         <v>48.4</v>
       </c>
       <c r="J497">
@@ -25577,7 +25580,7 @@
       <c r="H498">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I498">
+      <c r="I498" s="2">
         <v>28.27</v>
       </c>
       <c r="J498">
@@ -25618,7 +25621,7 @@
       <c r="H499">
         <v>0.16</v>
       </c>
-      <c r="I499">
+      <c r="I499" s="2">
         <v>16.05</v>
       </c>
       <c r="J499">
@@ -25659,7 +25662,7 @@
       <c r="H500">
         <v>0.34</v>
       </c>
-      <c r="I500">
+      <c r="I500" s="2">
         <v>34.14</v>
       </c>
       <c r="J500">
@@ -25700,7 +25703,7 @@
       <c r="H501">
         <v>0.22</v>
       </c>
-      <c r="I501">
+      <c r="I501" s="2">
         <v>22.42</v>
       </c>
       <c r="J501">
@@ -25741,7 +25744,7 @@
       <c r="H502">
         <v>0.42</v>
       </c>
-      <c r="I502">
+      <c r="I502" s="2">
         <v>41.67</v>
       </c>
       <c r="J502">
@@ -25782,7 +25785,7 @@
       <c r="H503">
         <v>0.26</v>
       </c>
-      <c r="I503">
+      <c r="I503" s="2">
         <v>26.15</v>
       </c>
       <c r="J503">
@@ -25823,7 +25826,7 @@
       <c r="H504">
         <v>0.31</v>
       </c>
-      <c r="I504">
+      <c r="I504" s="2">
         <v>30.82</v>
       </c>
       <c r="J504">
@@ -25864,7 +25867,7 @@
       <c r="H505">
         <v>0.3</v>
       </c>
-      <c r="I505">
+      <c r="I505" s="2">
         <v>29.56</v>
       </c>
       <c r="J505">
@@ -25905,7 +25908,7 @@
       <c r="H506">
         <v>0</v>
       </c>
-      <c r="I506">
+      <c r="I506" s="2">
         <v>0</v>
       </c>
       <c r="J506">
@@ -25940,7 +25943,7 @@
       <c r="H507">
         <v>0.2</v>
       </c>
-      <c r="I507">
+      <c r="I507" s="2">
         <v>20.329999999999998</v>
       </c>
       <c r="J507">
@@ -25981,7 +25984,7 @@
       <c r="H508">
         <v>0.39</v>
       </c>
-      <c r="I508">
+      <c r="I508" s="2">
         <v>39.06</v>
       </c>
       <c r="J508">
@@ -26022,7 +26025,7 @@
       <c r="H509">
         <v>0.36</v>
       </c>
-      <c r="I509">
+      <c r="I509" s="2">
         <v>36.43</v>
       </c>
       <c r="J509">
@@ -26063,7 +26066,7 @@
       <c r="H510">
         <v>0.31</v>
       </c>
-      <c r="I510">
+      <c r="I510" s="2">
         <v>31.31</v>
       </c>
       <c r="J510">
@@ -26104,7 +26107,7 @@
       <c r="H511">
         <v>0</v>
       </c>
-      <c r="I511">
+      <c r="I511" s="2">
         <v>0</v>
       </c>
       <c r="J511">
@@ -26139,7 +26142,7 @@
       <c r="H512">
         <v>0.36</v>
       </c>
-      <c r="I512">
+      <c r="I512" s="2">
         <v>36.130000000000003</v>
       </c>
       <c r="J512">
@@ -26180,7 +26183,7 @@
       <c r="H513">
         <v>0</v>
       </c>
-      <c r="I513">
+      <c r="I513" s="2">
         <v>0</v>
       </c>
       <c r="J513">
@@ -26215,7 +26218,7 @@
       <c r="H514">
         <v>0.43</v>
       </c>
-      <c r="I514">
+      <c r="I514" s="2">
         <v>42.78</v>
       </c>
       <c r="J514">
@@ -26256,7 +26259,7 @@
       <c r="H515">
         <v>0.35</v>
       </c>
-      <c r="I515">
+      <c r="I515" s="2">
         <v>34.67</v>
       </c>
       <c r="J515">
@@ -26297,7 +26300,7 @@
       <c r="H516">
         <v>0.39</v>
       </c>
-      <c r="I516">
+      <c r="I516" s="2">
         <v>38.54</v>
       </c>
       <c r="J516">
@@ -26338,7 +26341,7 @@
       <c r="H517">
         <v>0.25</v>
       </c>
-      <c r="I517">
+      <c r="I517" s="2">
         <v>25.35</v>
       </c>
       <c r="J517">
@@ -26379,7 +26382,7 @@
       <c r="H518">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I518">
+      <c r="I518" s="2">
         <v>28.61</v>
       </c>
       <c r="J518">
@@ -26420,7 +26423,7 @@
       <c r="H519">
         <v>0.22</v>
       </c>
-      <c r="I519">
+      <c r="I519" s="2">
         <v>22.49</v>
       </c>
       <c r="J519">
@@ -26461,7 +26464,7 @@
       <c r="H520">
         <v>0</v>
       </c>
-      <c r="I520">
+      <c r="I520" s="2">
         <v>0</v>
       </c>
       <c r="J520">
@@ -26496,7 +26499,7 @@
       <c r="H521">
         <v>0.42</v>
       </c>
-      <c r="I521">
+      <c r="I521" s="2">
         <v>41.62</v>
       </c>
       <c r="J521">
@@ -26537,7 +26540,7 @@
       <c r="H522">
         <v>0.2</v>
       </c>
-      <c r="I522">
+      <c r="I522" s="2">
         <v>19.93</v>
       </c>
       <c r="J522">
@@ -26578,7 +26581,7 @@
       <c r="H523">
         <v>0.31</v>
       </c>
-      <c r="I523">
+      <c r="I523" s="2">
         <v>30.66</v>
       </c>
       <c r="J523">

</xml_diff>